<commit_message>
Add paper PDF and update timeseries
</commit_message>
<xml_diff>
--- a/data/Time_series_COVID-19_GTA_github.xlsx
+++ b/data/Time_series_COVID-19_GTA_github.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\covid-GTA-surge-planning\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\covid-GTA-surge-planning-reports\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{857186B8-4357-4727-9AA9-25512F325254}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D78CE59-B737-4B63-AB5D-547E665ED042}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2136" yWindow="240" windowWidth="11508" windowHeight="12072" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="144" yWindow="0" windowWidth="11508" windowHeight="12072" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Time series" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="65">
   <si>
     <t>Location</t>
   </si>
@@ -280,6 +280,27 @@
   <si>
     <t>Yiu K, Wang L, Mishra S. COVID-19 GTA cumulative time series. Available at: https://github.com/mishra-lab/covid-GTA-surge-planning/blob/master/data/Time_series_COVID-19_GTA_github.xlsx. [Access date].</t>
   </si>
+  <si>
+    <t>^905</t>
+  </si>
+  <si>
+    <t>^968</t>
+  </si>
+  <si>
+    <t>*3346</t>
+  </si>
+  <si>
+    <t>^1034</t>
+  </si>
+  <si>
+    <t>*3546</t>
+  </si>
+  <si>
+    <t>^1083</t>
+  </si>
+  <si>
+    <t>^1149</t>
+  </si>
 </sst>
 </file>
 
@@ -288,13 +309,48 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -413,9 +469,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -424,10 +480,10 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -435,21 +491,42 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4133,10 +4210,10 @@
   <dimension ref="A1:HW24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="BZ2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="CE2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="BN1" sqref="BN1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="CF2" sqref="CF2"/>
+      <selection pane="bottomRight" activeCell="CJ13" sqref="CJ13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4396,6 +4473,21 @@
       <c r="CE1" s="2">
         <v>43936</v>
       </c>
+      <c r="CF1" s="2">
+        <v>43937</v>
+      </c>
+      <c r="CG1" s="2">
+        <v>43938</v>
+      </c>
+      <c r="CH1" s="2">
+        <v>43939</v>
+      </c>
+      <c r="CI1" s="2">
+        <v>43940</v>
+      </c>
+      <c r="CJ1" s="2">
+        <v>43941</v>
+      </c>
     </row>
     <row r="2" spans="1:231" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -4646,6 +4738,21 @@
       </c>
       <c r="CE2" s="14">
         <v>2369</v>
+      </c>
+      <c r="CF2" s="13">
+        <v>2559</v>
+      </c>
+      <c r="CG2" s="13">
+        <v>2818</v>
+      </c>
+      <c r="CH2" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="CI2" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="CJ2" s="13">
+        <v>3682</v>
       </c>
     </row>
     <row r="3" spans="1:231" x14ac:dyDescent="0.3">
@@ -4670,6 +4777,8 @@
       <c r="BH3" s="6"/>
       <c r="BI3" s="6"/>
       <c r="BJ3" s="6"/>
+      <c r="CH3" s="24"/>
+      <c r="CI3" s="24"/>
     </row>
     <row r="4" spans="1:231" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -4851,9 +4960,26 @@
       <c r="CE4" s="4">
         <v>456</v>
       </c>
+      <c r="CF4" s="4">
+        <v>496</v>
+      </c>
+      <c r="CG4" s="4">
+        <v>531</v>
+      </c>
+      <c r="CH4" s="25">
+        <v>568</v>
+      </c>
+      <c r="CI4" s="25">
+        <v>621</v>
+      </c>
+      <c r="CJ4" s="4">
+        <v>672</v>
+      </c>
     </row>
     <row r="5" spans="1:231" x14ac:dyDescent="0.3">
       <c r="BP5" s="6"/>
+      <c r="CH5" s="24"/>
+      <c r="CI5" s="24"/>
     </row>
     <row r="6" spans="1:231" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -5013,9 +5139,26 @@
       <c r="CE6" s="4">
         <v>344</v>
       </c>
+      <c r="CF6" s="4">
+        <v>350</v>
+      </c>
+      <c r="CG6" s="4">
+        <v>359</v>
+      </c>
+      <c r="CH6" s="25">
+        <v>368</v>
+      </c>
+      <c r="CI6" s="25">
+        <v>380</v>
+      </c>
+      <c r="CJ6" s="4">
+        <v>383</v>
+      </c>
     </row>
     <row r="7" spans="1:231" x14ac:dyDescent="0.3">
       <c r="BP7" s="6"/>
+      <c r="CH7" s="24"/>
+      <c r="CI7" s="24"/>
     </row>
     <row r="8" spans="1:231" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -5187,9 +5330,26 @@
       <c r="CE8" s="4">
         <v>1156</v>
       </c>
+      <c r="CF8" s="4">
+        <v>1219</v>
+      </c>
+      <c r="CG8" s="4">
+        <v>1274</v>
+      </c>
+      <c r="CH8" s="25">
+        <v>1347</v>
+      </c>
+      <c r="CI8" s="25">
+        <v>1449</v>
+      </c>
+      <c r="CJ8" s="4">
+        <v>1665</v>
+      </c>
     </row>
     <row r="9" spans="1:231" x14ac:dyDescent="0.3">
       <c r="BP9" s="6"/>
+      <c r="CH9" s="24"/>
+      <c r="CI9" s="24"/>
     </row>
     <row r="10" spans="1:231" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
@@ -5375,11 +5535,21 @@
       <c r="CE10" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="CF10" s="9"/>
-      <c r="CG10" s="9"/>
-      <c r="CH10" s="9"/>
-      <c r="CI10" s="9"/>
-      <c r="CJ10" s="9"/>
+      <c r="CF10" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="CG10" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="CH10" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="CI10" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="CJ10" s="28" t="s">
+        <v>64</v>
+      </c>
       <c r="CK10" s="9"/>
       <c r="CL10" s="9"/>
       <c r="CM10" s="9"/>
@@ -5856,6 +6026,26 @@
         <f>CE2+CE4+CE6+CE8+883</f>
         <v>5208</v>
       </c>
+      <c r="CF12">
+        <f>CF2+CF4+CF6+CF8+905</f>
+        <v>5529</v>
+      </c>
+      <c r="CG12">
+        <f>CG2+CG4+CG6+CG8+968</f>
+        <v>5950</v>
+      </c>
+      <c r="CH12">
+        <f>3346+CH4+CH6+CH8+1034</f>
+        <v>6663</v>
+      </c>
+      <c r="CI12">
+        <f>3546+CI4+CI6+CI8+1083</f>
+        <v>7079</v>
+      </c>
+      <c r="CJ12">
+        <f>CJ2+CJ4+CJ6+CJ8+1149</f>
+        <v>7551</v>
+      </c>
     </row>
     <row r="14" spans="1:231" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">

</xml_diff>

<commit_message>
Updated time series Apr 23
</commit_message>
<xml_diff>
--- a/data/Time_series_COVID-19_GTA_github.xlsx
+++ b/data/Time_series_COVID-19_GTA_github.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\covid-GTA-surge-planning-newrepo\covid-GTA-surge-planning\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{020BF8C7-6930-4C11-B791-39426C8396C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FF5F397-AF1B-4606-BC49-18C59F629706}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="144" yWindow="0" windowWidth="11508" windowHeight="12072" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="36" yWindow="12" windowWidth="11508" windowHeight="12072" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Time series" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="68">
   <si>
     <t>Location</t>
   </si>
@@ -304,6 +304,12 @@
   <si>
     <t>^1200</t>
   </si>
+  <si>
+    <t>*1963</t>
+  </si>
+  <si>
+    <t>^1250</t>
+  </si>
 </sst>
 </file>
 
@@ -312,13 +318,20 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -479,9 +492,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -490,10 +503,10 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -501,31 +514,34 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -4226,7 +4242,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="CI2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="BN1" sqref="BN1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="CK13" sqref="CK13"/>
+      <selection pane="bottomRight" activeCell="CL13" sqref="CL13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4504,6 +4520,9 @@
       <c r="CK1" s="2">
         <v>43942</v>
       </c>
+      <c r="CL1" s="2">
+        <v>43943</v>
+      </c>
     </row>
     <row r="2" spans="1:231" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -4772,6 +4791,9 @@
       </c>
       <c r="CK2" s="13">
         <v>3462</v>
+      </c>
+      <c r="CL2" s="13">
+        <v>3685</v>
       </c>
     </row>
     <row r="3" spans="1:231" x14ac:dyDescent="0.3">
@@ -4996,6 +5018,9 @@
       </c>
       <c r="CK4" s="4">
         <v>712</v>
+      </c>
+      <c r="CL4" s="4">
+        <v>757</v>
       </c>
     </row>
     <row r="5" spans="1:231" x14ac:dyDescent="0.3">
@@ -5179,6 +5204,9 @@
       <c r="CK6" s="4">
         <v>386</v>
       </c>
+      <c r="CL6" s="4">
+        <v>394</v>
+      </c>
     </row>
     <row r="7" spans="1:231" x14ac:dyDescent="0.3">
       <c r="BP7" s="6"/>
@@ -5373,6 +5401,9 @@
       <c r="CK8" s="4">
         <v>1752</v>
       </c>
+      <c r="CL8" s="13" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="9" spans="1:231" x14ac:dyDescent="0.3">
       <c r="BP9" s="6"/>
@@ -5581,7 +5612,9 @@
       <c r="CK10" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="CL10" s="9"/>
+      <c r="CL10" s="30" t="s">
+        <v>67</v>
+      </c>
       <c r="CM10" s="9"/>
       <c r="CN10" s="9"/>
       <c r="CO10" s="9"/>
@@ -6080,6 +6113,10 @@
         <f>CK2+CK4+CK6+CK8+1200</f>
         <v>7512</v>
       </c>
+      <c r="CL12">
+        <f>CL2+CL4+CL6+1963+1250</f>
+        <v>8049</v>
+      </c>
     </row>
     <row r="14" spans="1:231" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">

</xml_diff>

<commit_message>
Updated time series Apr 25
</commit_message>
<xml_diff>
--- a/data/Time_series_COVID-19_GTA_github.xlsx
+++ b/data/Time_series_COVID-19_GTA_github.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\covid-GTA-surge-planning-newrepo\covid-GTA-surge-planning\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75B8AA83-ADC8-4EC6-B9FF-F881D640A9AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BF361D9-295E-4760-8089-11A059964BAC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11508" windowHeight="12072" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Time series" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="71">
   <si>
     <t>Location</t>
   </si>
@@ -313,6 +313,12 @@
   <si>
     <t>^1278</t>
   </si>
+  <si>
+    <t>*2115</t>
+  </si>
+  <si>
+    <t>^1342</t>
+  </si>
 </sst>
 </file>
 
@@ -321,13 +327,20 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -502,9 +515,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -513,10 +526,10 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -524,31 +537,34 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1272,6 +1288,174 @@
       <xdr:spPr>
         <a:xfrm rot="19795862">
           <a:off x="42317699" y="714382"/>
+          <a:ext cx="3090270" cy="888641"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr>
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="5400" b="1" strike="noStrike" spc="-1">
+              <a:solidFill>
+                <a:srgbClr val="7C7C7C">
+                  <a:alpha val="50000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:latin typeface="Times New Roman"/>
+            </a:rPr>
+            <a:t>DRAFT</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="5400" b="0" strike="noStrike" spc="-1">
+            <a:solidFill>
+              <a:srgbClr val="7C7C7C">
+                <a:alpha val="50000"/>
+              </a:srgbClr>
+            </a:solidFill>
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>77</xdr:col>
+      <xdr:colOff>388649</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>171457</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>82</xdr:col>
+      <xdr:colOff>526169</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>155223</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="17" name="CustomShape 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1E0C8C74-5DE7-4BC3-A981-D207E5473663}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="19795862">
+          <a:off x="48242249" y="714382"/>
+          <a:ext cx="3090270" cy="888641"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr>
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="5400" b="1" strike="noStrike" spc="-1">
+              <a:solidFill>
+                <a:srgbClr val="7C7C7C">
+                  <a:alpha val="50000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:latin typeface="Times New Roman"/>
+            </a:rPr>
+            <a:t>DRAFT</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="5400" b="0" strike="noStrike" spc="-1">
+            <a:solidFill>
+              <a:srgbClr val="7C7C7C">
+                <a:alpha val="50000"/>
+              </a:srgbClr>
+            </a:solidFill>
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>87</xdr:col>
+      <xdr:colOff>188623</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>171456</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>92</xdr:col>
+      <xdr:colOff>326143</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>155222</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="18" name="CustomShape 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6DEFD677-B910-4710-8B46-C158DFE35CB9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="19795862">
+          <a:off x="53947723" y="714381"/>
           <a:ext cx="3090270" cy="888641"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4252,10 +4436,10 @@
   <dimension ref="A1:HW23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="CE2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="BU2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="BN1" sqref="BN1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="CI23" sqref="CI23"/>
+      <selection pane="bottomRight" activeCell="CL19" sqref="CL19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4539,6 +4723,9 @@
       <c r="CM1" s="2">
         <v>43944</v>
       </c>
+      <c r="CN1" s="2">
+        <v>43945</v>
+      </c>
     </row>
     <row r="2" spans="1:231" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -4813,6 +5000,9 @@
       </c>
       <c r="CM2" s="13">
         <v>3933</v>
+      </c>
+      <c r="CN2" s="13">
+        <v>4048</v>
       </c>
     </row>
     <row r="3" spans="1:231" x14ac:dyDescent="0.3">
@@ -5043,6 +5233,9 @@
       </c>
       <c r="CM4" s="4">
         <v>781</v>
+      </c>
+      <c r="CN4" s="4">
+        <v>810</v>
       </c>
     </row>
     <row r="5" spans="1:231" x14ac:dyDescent="0.3">
@@ -5232,6 +5425,9 @@
       <c r="CM6" s="4">
         <v>410</v>
       </c>
+      <c r="CN6" s="4">
+        <v>415</v>
+      </c>
     </row>
     <row r="7" spans="1:231" x14ac:dyDescent="0.3">
       <c r="BP7" s="6"/>
@@ -5432,6 +5628,9 @@
       <c r="CM8" s="13" t="s">
         <v>67</v>
       </c>
+      <c r="CN8" s="13" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="9" spans="1:231" x14ac:dyDescent="0.3">
       <c r="BP9" s="6"/>
@@ -5646,7 +5845,9 @@
       <c r="CM10" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="CN10" s="9"/>
+      <c r="CN10" s="32" t="s">
+        <v>70</v>
+      </c>
       <c r="CO10" s="9"/>
       <c r="CP10" s="9"/>
       <c r="CQ10" s="9"/>

</xml_diff>

<commit_message>
Time series update Apr 26
</commit_message>
<xml_diff>
--- a/data/Time_series_COVID-19_GTA_github.xlsx
+++ b/data/Time_series_COVID-19_GTA_github.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\covid-GTA-surge-planning-newrepo\covid-GTA-surge-planning\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BF361D9-295E-4760-8089-11A059964BAC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F393017-7B8A-44D3-AA33-071D3F3D1988}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11532" yWindow="288" windowWidth="11508" windowHeight="12072" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Time series" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="74">
   <si>
     <t>Location</t>
   </si>
@@ -319,6 +319,15 @@
   <si>
     <t>^1342</t>
   </si>
+  <si>
+    <t>*4628</t>
+  </si>
+  <si>
+    <t>*2175</t>
+  </si>
+  <si>
+    <t>^1387</t>
+  </si>
 </sst>
 </file>
 
@@ -327,13 +336,20 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm"/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -515,9 +531,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -526,10 +542,10 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -537,31 +553,34 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1433,14 +1452,14 @@
     <xdr:from>
       <xdr:col>87</xdr:col>
       <xdr:colOff>188623</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>171456</xdr:rowOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>6</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>92</xdr:col>
       <xdr:colOff>326143</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>155222</xdr:rowOff>
+      <xdr:rowOff>164747</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1455,7 +1474,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="19795862">
-          <a:off x="53947723" y="714381"/>
+          <a:off x="53947723" y="723906"/>
           <a:ext cx="3090270" cy="888641"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4436,10 +4455,10 @@
   <dimension ref="A1:HW23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="BU2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="CJ2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="BN1" sqref="BN1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="CL19" sqref="CL19"/>
+      <selection pane="bottomRight" activeCell="CO10" sqref="CO10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4726,6 +4745,9 @@
       <c r="CN1" s="2">
         <v>43945</v>
       </c>
+      <c r="CO1" s="2">
+        <v>43946</v>
+      </c>
     </row>
     <row r="2" spans="1:231" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -5003,6 +5025,9 @@
       </c>
       <c r="CN2" s="13">
         <v>4048</v>
+      </c>
+      <c r="CO2" s="13" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:231" x14ac:dyDescent="0.3">
@@ -5236,6 +5261,9 @@
       </c>
       <c r="CN4" s="4">
         <v>810</v>
+      </c>
+      <c r="CO4" s="4">
+        <v>836</v>
       </c>
     </row>
     <row r="5" spans="1:231" x14ac:dyDescent="0.3">
@@ -5428,6 +5456,9 @@
       <c r="CN6" s="4">
         <v>415</v>
       </c>
+      <c r="CO6" s="4">
+        <v>418</v>
+      </c>
     </row>
     <row r="7" spans="1:231" x14ac:dyDescent="0.3">
       <c r="BP7" s="6"/>
@@ -5631,6 +5662,9 @@
       <c r="CN8" s="13" t="s">
         <v>69</v>
       </c>
+      <c r="CO8" s="13" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="9" spans="1:231" x14ac:dyDescent="0.3">
       <c r="BP9" s="6"/>
@@ -5848,7 +5882,9 @@
       <c r="CN10" s="32" t="s">
         <v>70</v>
       </c>
-      <c r="CO10" s="9"/>
+      <c r="CO10" s="33" t="s">
+        <v>73</v>
+      </c>
       <c r="CP10" s="9"/>
       <c r="CQ10" s="9"/>
       <c r="CR10" s="9"/>

</xml_diff>

<commit_message>
Updated time series Apr 26
</commit_message>
<xml_diff>
--- a/data/Time_series_COVID-19_GTA_github.xlsx
+++ b/data/Time_series_COVID-19_GTA_github.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\covid-GTA-surge-planning-newrepo\covid-GTA-surge-planning\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F393017-7B8A-44D3-AA33-071D3F3D1988}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E58A23D8-6806-4ADD-B7D6-6F44FD126590}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11532" yWindow="288" windowWidth="11508" windowHeight="12072" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="77">
   <si>
     <t>Location</t>
   </si>
@@ -328,6 +328,15 @@
   <si>
     <t>^1387</t>
   </si>
+  <si>
+    <t>*4798</t>
+  </si>
+  <si>
+    <t>*2267</t>
+  </si>
+  <si>
+    <t>^1405</t>
+  </si>
 </sst>
 </file>
 
@@ -336,13 +345,20 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -531,9 +547,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -542,10 +558,10 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -553,31 +569,34 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -4458,7 +4477,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="CJ2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="BN1" sqref="BN1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="CO10" sqref="CO10"/>
+      <selection pane="bottomRight" activeCell="CP10" sqref="CP10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4748,6 +4767,9 @@
       <c r="CO1" s="2">
         <v>43946</v>
       </c>
+      <c r="CP1" s="2">
+        <v>43947</v>
+      </c>
     </row>
     <row r="2" spans="1:231" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -5028,6 +5050,9 @@
       </c>
       <c r="CO2" s="13" t="s">
         <v>71</v>
+      </c>
+      <c r="CP2" s="13" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:231" x14ac:dyDescent="0.3">
@@ -5264,6 +5289,9 @@
       </c>
       <c r="CO4" s="4">
         <v>836</v>
+      </c>
+      <c r="CP4" s="4">
+        <v>875</v>
       </c>
     </row>
     <row r="5" spans="1:231" x14ac:dyDescent="0.3">
@@ -5459,6 +5487,9 @@
       <c r="CO6" s="4">
         <v>418</v>
       </c>
+      <c r="CP6" s="4">
+        <v>422</v>
+      </c>
     </row>
     <row r="7" spans="1:231" x14ac:dyDescent="0.3">
       <c r="BP7" s="6"/>
@@ -5665,6 +5696,9 @@
       <c r="CO8" s="13" t="s">
         <v>72</v>
       </c>
+      <c r="CP8" s="13" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="9" spans="1:231" x14ac:dyDescent="0.3">
       <c r="BP9" s="6"/>
@@ -5885,7 +5919,9 @@
       <c r="CO10" s="33" t="s">
         <v>73</v>
       </c>
-      <c r="CP10" s="9"/>
+      <c r="CP10" s="34" t="s">
+        <v>76</v>
+      </c>
       <c r="CQ10" s="9"/>
       <c r="CR10" s="9"/>
       <c r="CS10" s="9"/>

</xml_diff>

<commit_message>
Time series updated Apr 28
</commit_message>
<xml_diff>
--- a/data/Time_series_COVID-19_GTA_github.xlsx
+++ b/data/Time_series_COVID-19_GTA_github.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\covid-GTA-surge-planning-newrepo\covid-GTA-surge-planning\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E58A23D8-6806-4ADD-B7D6-6F44FD126590}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48C6F24C-B4D5-4773-883A-7661739255F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11532" yWindow="288" windowWidth="11508" windowHeight="12072" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="108" yWindow="96" windowWidth="11508" windowHeight="12072" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Time series" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="66">
   <si>
     <t>Location</t>
   </si>
@@ -120,18 +120,6 @@
     <t>Please use the following recommended citation for this dataset:</t>
   </si>
   <si>
-    <t>*1891</t>
-  </si>
-  <si>
-    <t>*Includes confirmed and probable cases</t>
-  </si>
-  <si>
-    <t>*2065</t>
-  </si>
-  <si>
-    <t>*2225</t>
-  </si>
-  <si>
     <t>^212</t>
   </si>
   <si>
@@ -187,28 +175,6 @@
   </si>
   <si>
     <t>^225</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Note: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>All data, unless otherwise specified, are based on reported date of confirmed cases</t>
-    </r>
   </si>
   <si>
     <t>^Cases reported based on accurate episode date</t>
@@ -284,15 +250,9 @@
     <t>^968</t>
   </si>
   <si>
-    <t>*3346</t>
-  </si>
-  <si>
     <t>^1034</t>
   </si>
   <si>
-    <t>*3546</t>
-  </si>
-  <si>
     <t>^1083</t>
   </si>
   <si>
@@ -302,40 +262,58 @@
     <t>^1200</t>
   </si>
   <si>
-    <t>*1963</t>
-  </si>
-  <si>
     <t>^1250</t>
   </si>
   <si>
-    <t>*2030</t>
-  </si>
-  <si>
     <t>^1278</t>
   </si>
   <si>
-    <t>*2115</t>
-  </si>
-  <si>
     <t>^1342</t>
   </si>
   <si>
-    <t>*4628</t>
-  </si>
-  <si>
-    <t>*2175</t>
-  </si>
-  <si>
     <t>^1387</t>
   </si>
   <si>
-    <t>*4798</t>
-  </si>
-  <si>
-    <t>*2267</t>
-  </si>
-  <si>
     <t>^1405</t>
+  </si>
+  <si>
+    <t>^1430</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Note 1: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>All data, unless otherwise specified, are based on reported date of confirmed cases</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Note 2: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>There are gaps in the City of Toronto (e.g., Apr 10-12) and Peel Region (Apr 22 onward) time series as the governments did not report number of confirmed cases on those days, only total number of confirmed and probable cases</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -345,13 +323,20 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -480,7 +465,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -525,12 +510,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor rgb="FF7C7C7C"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -547,9 +526,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -558,42 +537,42 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -619,6 +598,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -4474,10 +4459,10 @@
   <dimension ref="A1:HW23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="CJ2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="CF2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="BN1" sqref="BN1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="CP10" sqref="CP10"/>
+      <selection pane="bottomRight" activeCell="CF20" sqref="CF20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4770,6 +4755,9 @@
       <c r="CP1" s="2">
         <v>43947</v>
       </c>
+      <c r="CQ1" s="2">
+        <v>43948</v>
+      </c>
     </row>
     <row r="2" spans="1:231" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -4901,34 +4889,34 @@
       <c r="AQ2" s="4">
         <v>14</v>
       </c>
-      <c r="AR2" s="21">
+      <c r="AR2" s="20">
         <v>14</v>
       </c>
-      <c r="AS2" s="21">
+      <c r="AS2" s="20">
         <v>19</v>
       </c>
-      <c r="AT2" s="21">
+      <c r="AT2" s="20">
         <v>22</v>
       </c>
-      <c r="AU2" s="21">
+      <c r="AU2" s="20">
         <v>30</v>
       </c>
-      <c r="AV2" s="21">
+      <c r="AV2" s="20">
         <v>51</v>
       </c>
-      <c r="AW2" s="21">
+      <c r="AW2" s="20">
         <v>65</v>
       </c>
-      <c r="AX2" s="21">
+      <c r="AX2" s="20">
         <v>76</v>
       </c>
-      <c r="AY2" s="21">
+      <c r="AY2" s="20">
         <v>79</v>
       </c>
-      <c r="AZ2" s="21">
+      <c r="AZ2" s="20">
         <v>89</v>
       </c>
-      <c r="BA2" s="21">
+      <c r="BA2" s="20">
         <v>91</v>
       </c>
       <c r="BB2" s="4">
@@ -5003,56 +4991,45 @@
       <c r="BY2" s="4">
         <v>1519</v>
       </c>
-      <c r="BZ2" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="CA2" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="CB2" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="CC2" s="13">
+      <c r="BZ2" s="34"/>
+      <c r="CA2" s="34"/>
+      <c r="CB2" s="34"/>
+      <c r="CC2" s="12">
         <v>2088</v>
       </c>
-      <c r="CD2" s="14">
+      <c r="CD2" s="13">
         <v>2257</v>
       </c>
-      <c r="CE2" s="14">
+      <c r="CE2" s="13">
         <v>2369</v>
       </c>
-      <c r="CF2" s="13">
+      <c r="CF2" s="12">
         <v>2559</v>
       </c>
-      <c r="CG2" s="13">
+      <c r="CG2" s="12">
         <v>2818</v>
       </c>
-      <c r="CH2" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="CI2" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="CJ2" s="13">
+      <c r="CH2" s="34"/>
+      <c r="CI2" s="34"/>
+      <c r="CJ2" s="12">
         <v>3343</v>
       </c>
-      <c r="CK2" s="13">
+      <c r="CK2" s="12">
         <v>3462</v>
       </c>
-      <c r="CL2" s="13">
+      <c r="CL2" s="12">
         <v>3685</v>
       </c>
-      <c r="CM2" s="13">
+      <c r="CM2" s="12">
         <v>3933</v>
       </c>
-      <c r="CN2" s="13">
+      <c r="CN2" s="12">
         <v>4048</v>
       </c>
-      <c r="CO2" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="CP2" s="13" t="s">
-        <v>74</v>
+      <c r="CO2" s="34"/>
+      <c r="CP2" s="34"/>
+      <c r="CQ2" s="12">
+        <v>4493</v>
       </c>
     </row>
     <row r="3" spans="1:231" x14ac:dyDescent="0.3">
@@ -5077,8 +5054,8 @@
       <c r="BH3" s="6"/>
       <c r="BI3" s="6"/>
       <c r="BJ3" s="6"/>
-      <c r="CH3" s="24"/>
-      <c r="CI3" s="24"/>
+      <c r="CH3" s="23"/>
+      <c r="CI3" s="23"/>
     </row>
     <row r="4" spans="1:231" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -5266,10 +5243,10 @@
       <c r="CG4" s="4">
         <v>531</v>
       </c>
-      <c r="CH4" s="25">
+      <c r="CH4" s="24">
         <v>568</v>
       </c>
-      <c r="CI4" s="25">
+      <c r="CI4" s="24">
         <v>621</v>
       </c>
       <c r="CJ4" s="4">
@@ -5292,12 +5269,15 @@
       </c>
       <c r="CP4" s="4">
         <v>875</v>
+      </c>
+      <c r="CQ4" s="4">
+        <v>899</v>
       </c>
     </row>
     <row r="5" spans="1:231" x14ac:dyDescent="0.3">
       <c r="BP5" s="6"/>
-      <c r="CH5" s="24"/>
-      <c r="CI5" s="24"/>
+      <c r="CH5" s="23"/>
+      <c r="CI5" s="23"/>
     </row>
     <row r="6" spans="1:231" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -5463,10 +5443,10 @@
       <c r="CG6" s="4">
         <v>359</v>
       </c>
-      <c r="CH6" s="25">
+      <c r="CH6" s="24">
         <v>368</v>
       </c>
-      <c r="CI6" s="25">
+      <c r="CI6" s="24">
         <v>380</v>
       </c>
       <c r="CJ6" s="4">
@@ -5489,12 +5469,15 @@
       </c>
       <c r="CP6" s="4">
         <v>422</v>
+      </c>
+      <c r="CQ6" s="4">
+        <v>429</v>
       </c>
     </row>
     <row r="7" spans="1:231" x14ac:dyDescent="0.3">
       <c r="BP7" s="6"/>
-      <c r="CH7" s="24"/>
-      <c r="CI7" s="24"/>
+      <c r="CH7" s="23"/>
+      <c r="CI7" s="23"/>
     </row>
     <row r="8" spans="1:231" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -5672,10 +5655,10 @@
       <c r="CG8" s="4">
         <v>1274</v>
       </c>
-      <c r="CH8" s="25">
+      <c r="CH8" s="24">
         <v>1347</v>
       </c>
-      <c r="CI8" s="25">
+      <c r="CI8" s="24">
         <v>1449</v>
       </c>
       <c r="CJ8" s="4">
@@ -5684,26 +5667,16 @@
       <c r="CK8" s="4">
         <v>1752</v>
       </c>
-      <c r="CL8" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="CM8" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="CN8" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="CO8" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="CP8" s="13" t="s">
-        <v>75</v>
-      </c>
+      <c r="CL8" s="34"/>
+      <c r="CM8" s="34"/>
+      <c r="CN8" s="34"/>
+      <c r="CO8" s="34"/>
+      <c r="CP8" s="34"/>
     </row>
     <row r="9" spans="1:231" x14ac:dyDescent="0.3">
       <c r="BP9" s="6"/>
-      <c r="CH9" s="24"/>
-      <c r="CI9" s="24"/>
+      <c r="CH9" s="23"/>
+      <c r="CI9" s="23"/>
     </row>
     <row r="10" spans="1:231" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
@@ -5742,187 +5715,189 @@
       <c r="AF10" s="10"/>
       <c r="AG10" s="10"/>
       <c r="AH10" s="10"/>
-      <c r="AI10" s="14">
+      <c r="AI10" s="13">
         <v>1</v>
       </c>
-      <c r="AJ10" s="14">
+      <c r="AJ10" s="13">
         <v>3</v>
       </c>
-      <c r="AK10" s="14">
+      <c r="AK10" s="13">
         <v>6</v>
       </c>
-      <c r="AL10" s="14">
+      <c r="AL10" s="13">
         <v>6</v>
       </c>
-      <c r="AM10" s="14">
+      <c r="AM10" s="13">
         <v>6</v>
       </c>
-      <c r="AN10" s="14">
+      <c r="AN10" s="13">
         <v>6</v>
       </c>
-      <c r="AO10" s="14">
+      <c r="AO10" s="13">
         <v>6</v>
       </c>
-      <c r="AP10" s="14">
+      <c r="AP10" s="13">
         <v>6</v>
       </c>
-      <c r="AQ10" s="14">
+      <c r="AQ10" s="13">
         <v>7</v>
       </c>
-      <c r="AR10" s="14">
+      <c r="AR10" s="13">
         <v>7</v>
       </c>
-      <c r="AS10" s="14">
+      <c r="AS10" s="13">
         <v>7</v>
       </c>
-      <c r="AT10" s="14">
+      <c r="AT10" s="13">
         <v>8</v>
       </c>
-      <c r="AU10" s="14">
+      <c r="AU10" s="13">
         <v>9</v>
       </c>
-      <c r="AV10" s="14">
+      <c r="AV10" s="13">
         <v>9</v>
       </c>
-      <c r="AW10" s="14">
+      <c r="AW10" s="13">
         <v>11</v>
       </c>
-      <c r="AX10" s="14">
+      <c r="AX10" s="13">
         <v>11</v>
       </c>
-      <c r="AY10" s="14">
+      <c r="AY10" s="13">
         <v>16</v>
       </c>
-      <c r="AZ10" s="14">
+      <c r="AZ10" s="13">
         <v>20</v>
       </c>
-      <c r="BA10" s="14">
+      <c r="BA10" s="13">
         <v>27</v>
       </c>
-      <c r="BB10" s="14">
+      <c r="BB10" s="13">
         <v>28</v>
       </c>
-      <c r="BC10" s="14">
+      <c r="BC10" s="13">
         <v>32</v>
       </c>
-      <c r="BD10" s="14">
+      <c r="BD10" s="13">
         <v>36</v>
       </c>
-      <c r="BE10" s="17">
+      <c r="BE10" s="16">
         <v>43</v>
       </c>
-      <c r="BF10" s="14">
+      <c r="BF10" s="13">
         <v>48</v>
       </c>
-      <c r="BG10" s="14">
+      <c r="BG10" s="13">
         <v>54</v>
       </c>
-      <c r="BH10" s="14">
+      <c r="BH10" s="13">
         <v>59</v>
       </c>
-      <c r="BI10" s="14">
+      <c r="BI10" s="13">
         <v>97</v>
       </c>
-      <c r="BJ10" s="14">
+      <c r="BJ10" s="13">
         <v>110</v>
       </c>
       <c r="BK10" s="11">
         <v>185</v>
       </c>
-      <c r="BL10" s="15" t="s">
+      <c r="BL10" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="BM10" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="BN10" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="BO10" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="BP10" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="BQ10" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="BR10" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="BS10" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="BT10" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="BU10" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="BV10" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="BW10" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="BX10" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="BY10" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="BZ10" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="CA10" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="BM10" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="BN10" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="BO10" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="BP10" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="BQ10" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="BR10" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="BS10" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="BT10" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="BU10" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="BV10" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="BW10" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="BX10" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="BY10" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="BZ10" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="CA10" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="CB10" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="CC10" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="CD10" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="CE10" s="20" t="s">
+      <c r="CB10" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="CC10" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="CD10" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="CE10" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="CF10" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="CG10" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="CH10" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="CI10" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="CF10" s="22" t="s">
+      <c r="CJ10" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="CK10" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="CG10" s="23" t="s">
+      <c r="CL10" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="CH10" s="26" t="s">
+      <c r="CM10" s="30" t="s">
+        <v>59</v>
+      </c>
+      <c r="CN10" s="31" t="s">
         <v>60</v>
       </c>
-      <c r="CI10" s="27" t="s">
+      <c r="CO10" s="32" t="s">
+        <v>61</v>
+      </c>
+      <c r="CP10" s="33" t="s">
         <v>62</v>
       </c>
-      <c r="CJ10" s="28" t="s">
+      <c r="CQ10" s="36" t="s">
         <v>63</v>
       </c>
-      <c r="CK10" s="29" t="s">
-        <v>64</v>
-      </c>
-      <c r="CL10" s="30" t="s">
-        <v>66</v>
-      </c>
-      <c r="CM10" s="31" t="s">
-        <v>68</v>
-      </c>
-      <c r="CN10" s="32" t="s">
-        <v>70</v>
-      </c>
-      <c r="CO10" s="33" t="s">
-        <v>73</v>
-      </c>
-      <c r="CP10" s="34" t="s">
-        <v>76</v>
-      </c>
-      <c r="CQ10" s="9"/>
       <c r="CR10" s="9"/>
       <c r="CS10" s="9"/>
       <c r="CT10" s="9"/>
@@ -6086,32 +6061,32 @@
       </c>
     </row>
     <row r="19" spans="1:1" s="6" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A19" s="16" t="s">
-        <v>50</v>
+      <c r="A19" s="15" t="s">
+        <v>64</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>28</v>
+    <row r="20" spans="1:1" ht="72" x14ac:dyDescent="0.3">
+      <c r="A20" s="35" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="23" spans="1:1" ht="228" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="18" t="s">
-        <v>54</v>
+      <c r="A23" s="17" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;CDRAFT]</oddHeader>
   </headerFooter>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -6200,8 +6175,8 @@
       </c>
     </row>
     <row r="5" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="19" t="s">
-        <v>52</v>
+      <c r="B5" s="18" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -6254,7 +6229,7 @@
         <v>25</v>
       </c>
       <c r="B18" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -6283,7 +6258,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated time series Apr 29
</commit_message>
<xml_diff>
--- a/data/Time_series_COVID-19_GTA_github.xlsx
+++ b/data/Time_series_COVID-19_GTA_github.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\covid-GTA-surge-planning-newrepo\covid-GTA-surge-planning\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48C6F24C-B4D5-4773-883A-7661739255F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D52D8233-8D13-4131-B435-D99D17165A51}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="108" yWindow="96" windowWidth="11508" windowHeight="12072" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Time series" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="67">
   <si>
     <t>Location</t>
   </si>
@@ -315,6 +315,9 @@
       <t>There are gaps in the City of Toronto (e.g., Apr 10-12) and Peel Region (Apr 22 onward) time series as the governments did not report number of confirmed cases on those days, only total number of confirmed and probable cases</t>
     </r>
   </si>
+  <si>
+    <t>^1457</t>
+  </si>
 </sst>
 </file>
 
@@ -323,13 +326,20 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -526,9 +536,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -537,39 +547,42 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -596,14 +609,14 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -4459,10 +4472,10 @@
   <dimension ref="A1:HW23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="CF2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="CD2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="BN1" sqref="BN1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="CF20" sqref="CF20"/>
+      <selection pane="bottomRight" activeCell="CS10" sqref="CS10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4758,6 +4771,9 @@
       <c r="CQ1" s="2">
         <v>43948</v>
       </c>
+      <c r="CR1" s="2">
+        <v>43949</v>
+      </c>
     </row>
     <row r="2" spans="1:231" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -5030,6 +5046,9 @@
       <c r="CP2" s="34"/>
       <c r="CQ2" s="12">
         <v>4493</v>
+      </c>
+      <c r="CR2" s="12">
+        <v>4647</v>
       </c>
     </row>
     <row r="3" spans="1:231" x14ac:dyDescent="0.3">
@@ -5272,6 +5291,9 @@
       </c>
       <c r="CQ4" s="4">
         <v>899</v>
+      </c>
+      <c r="CR4" s="4">
+        <v>923</v>
       </c>
     </row>
     <row r="5" spans="1:231" x14ac:dyDescent="0.3">
@@ -5473,6 +5495,9 @@
       <c r="CQ6" s="4">
         <v>429</v>
       </c>
+      <c r="CR6" s="4">
+        <v>443</v>
+      </c>
     </row>
     <row r="7" spans="1:231" x14ac:dyDescent="0.3">
       <c r="BP7" s="6"/>
@@ -5898,7 +5923,9 @@
       <c r="CQ10" s="36" t="s">
         <v>63</v>
       </c>
-      <c r="CR10" s="9"/>
+      <c r="CR10" s="37" t="s">
+        <v>66</v>
+      </c>
       <c r="CS10" s="9"/>
       <c r="CT10" s="9"/>
       <c r="CU10" s="9"/>

</xml_diff>

<commit_message>
Updated time series Apr 30
</commit_message>
<xml_diff>
--- a/data/Time_series_COVID-19_GTA_github.xlsx
+++ b/data/Time_series_COVID-19_GTA_github.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\covid-GTA-surge-planning-newrepo\covid-GTA-surge-planning\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D52D8233-8D13-4131-B435-D99D17165A51}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82827866-936A-4748-8B2B-B7756455DDD0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,14 +19,12 @@
     <sheet name="References" sheetId="3" r:id="rId4"/>
     <sheet name="Recommended Citation" sheetId="4" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -37,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
   <si>
     <t>Location</t>
   </si>
@@ -120,66 +118,6 @@
     <t>Please use the following recommended citation for this dataset:</t>
   </si>
   <si>
-    <t>^212</t>
-  </si>
-  <si>
-    <t>^824</t>
-  </si>
-  <si>
-    <t>^765</t>
-  </si>
-  <si>
-    <t>^697</t>
-  </si>
-  <si>
-    <t>^679</t>
-  </si>
-  <si>
-    <t>^656</t>
-  </si>
-  <si>
-    <t>^604</t>
-  </si>
-  <si>
-    <t>^558</t>
-  </si>
-  <si>
-    <t>^523</t>
-  </si>
-  <si>
-    <t>^464</t>
-  </si>
-  <si>
-    <t>^452</t>
-  </si>
-  <si>
-    <t>^431</t>
-  </si>
-  <si>
-    <t>^407</t>
-  </si>
-  <si>
-    <t>^347</t>
-  </si>
-  <si>
-    <t>^325</t>
-  </si>
-  <si>
-    <t>^319</t>
-  </si>
-  <si>
-    <t>^293</t>
-  </si>
-  <si>
-    <t>^235</t>
-  </si>
-  <si>
-    <t>^225</t>
-  </si>
-  <si>
-    <t>^Cases reported based on accurate episode date</t>
-  </si>
-  <si>
     <r>
       <t>3. City of Toronto. COVID-19: Status of Cases in Toronto 2020 [Available from: https://www.toronto.ca/home/covid-19/media-room/covid-19-status-of-cases-in-toronto/</t>
     </r>
@@ -238,46 +176,21 @@
     </r>
   </si>
   <si>
-    <t>^883</t>
-  </si>
-  <si>
     <t>Yiu K, Wang L, Mishra S. COVID-19 GTA cumulative time series. Available at: https://github.com/mishra-lab/covid-GTA-surge-planning/blob/master/data/Time_series_COVID-19_GTA_github.xlsx. [Access date].</t>
   </si>
   <si>
-    <t>^905</t>
-  </si>
-  <si>
-    <t>^968</t>
-  </si>
-  <si>
-    <t>^1034</t>
-  </si>
-  <si>
-    <t>^1083</t>
-  </si>
-  <si>
-    <t>^1149</t>
-  </si>
-  <si>
-    <t>^1200</t>
-  </si>
-  <si>
-    <t>^1250</t>
-  </si>
-  <si>
-    <t>^1278</t>
-  </si>
-  <si>
-    <t>^1342</t>
-  </si>
-  <si>
-    <t>^1387</t>
-  </si>
-  <si>
-    <t>^1405</t>
-  </si>
-  <si>
-    <t>^1430</t>
+    <r>
+      <t xml:space="preserve">Note 2: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>There are gaps in the City of Toronto (e.g., Apr 10-12) and Peel Region (Apr 22 onward) time series as the governments did not report number of confirmed cases on those days, only total number of confirmed and probable cases</t>
+    </r>
   </si>
   <si>
     <r>
@@ -298,25 +211,8 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>All data, unless otherwise specified, are based on reported date of confirmed cases</t>
+      <t>All data are based on confirmed cases reported as of that day</t>
     </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Note 2: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>There are gaps in the City of Toronto (e.g., Apr 10-12) and Peel Region (Apr 22 onward) time series as the governments did not report number of confirmed cases on those days, only total number of confirmed and probable cases</t>
-    </r>
-  </si>
-  <si>
-    <t>^1457</t>
   </si>
 </sst>
 </file>
@@ -326,104 +222,13 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm"/>
   </numFmts>
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -534,11 +339,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -547,84 +353,41 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="2" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal_Time series" xfId="1" xr:uid="{A61095A3-42BD-48CB-9DCB-BF39FFF940A7}"/>
+    <cellStyle name="Normal_Time series_1" xfId="2" xr:uid="{A441D0D6-709F-4E84-8CCF-7AA0C0FD41F2}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -4469,13 +4232,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:HW23"/>
+  <dimension ref="A1:HW22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="CD2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="CI2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="BN1" sqref="BN1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="CS10" sqref="CS10"/>
+      <selection pane="bottomRight" activeCell="CN14" sqref="CN14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4774,6 +4537,9 @@
       <c r="CR1" s="2">
         <v>43949</v>
       </c>
+      <c r="CS1" s="2">
+        <v>43950</v>
+      </c>
     </row>
     <row r="2" spans="1:231" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -4905,34 +4671,34 @@
       <c r="AQ2" s="4">
         <v>14</v>
       </c>
-      <c r="AR2" s="20">
+      <c r="AR2" s="18">
         <v>14</v>
       </c>
-      <c r="AS2" s="20">
+      <c r="AS2" s="18">
         <v>19</v>
       </c>
-      <c r="AT2" s="20">
+      <c r="AT2" s="18">
         <v>22</v>
       </c>
-      <c r="AU2" s="20">
+      <c r="AU2" s="18">
         <v>30</v>
       </c>
-      <c r="AV2" s="20">
+      <c r="AV2" s="18">
         <v>51</v>
       </c>
-      <c r="AW2" s="20">
+      <c r="AW2" s="18">
         <v>65</v>
       </c>
-      <c r="AX2" s="20">
+      <c r="AX2" s="18">
         <v>76</v>
       </c>
-      <c r="AY2" s="20">
+      <c r="AY2" s="18">
         <v>79</v>
       </c>
-      <c r="AZ2" s="20">
+      <c r="AZ2" s="18">
         <v>89</v>
       </c>
-      <c r="BA2" s="20">
+      <c r="BA2" s="18">
         <v>91</v>
       </c>
       <c r="BB2" s="4">
@@ -5007,9 +4773,9 @@
       <c r="BY2" s="4">
         <v>1519</v>
       </c>
-      <c r="BZ2" s="34"/>
-      <c r="CA2" s="34"/>
-      <c r="CB2" s="34"/>
+      <c r="BZ2" s="21"/>
+      <c r="CA2" s="21"/>
+      <c r="CB2" s="21"/>
       <c r="CC2" s="12">
         <v>2088</v>
       </c>
@@ -5025,8 +4791,8 @@
       <c r="CG2" s="12">
         <v>2818</v>
       </c>
-      <c r="CH2" s="34"/>
-      <c r="CI2" s="34"/>
+      <c r="CH2" s="21"/>
+      <c r="CI2" s="21"/>
       <c r="CJ2" s="12">
         <v>3343</v>
       </c>
@@ -5042,13 +4808,16 @@
       <c r="CN2" s="12">
         <v>4048</v>
       </c>
-      <c r="CO2" s="34"/>
-      <c r="CP2" s="34"/>
+      <c r="CO2" s="21"/>
+      <c r="CP2" s="21"/>
       <c r="CQ2" s="12">
         <v>4493</v>
       </c>
       <c r="CR2" s="12">
         <v>4647</v>
+      </c>
+      <c r="CS2" s="12">
+        <v>4845</v>
       </c>
     </row>
     <row r="3" spans="1:231" x14ac:dyDescent="0.3">
@@ -5073,8 +4842,8 @@
       <c r="BH3" s="6"/>
       <c r="BI3" s="6"/>
       <c r="BJ3" s="6"/>
-      <c r="CH3" s="23"/>
-      <c r="CI3" s="23"/>
+      <c r="CH3" s="19"/>
+      <c r="CI3" s="19"/>
     </row>
     <row r="4" spans="1:231" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -5262,10 +5031,10 @@
       <c r="CG4" s="4">
         <v>531</v>
       </c>
-      <c r="CH4" s="24">
+      <c r="CH4" s="20">
         <v>568</v>
       </c>
-      <c r="CI4" s="24">
+      <c r="CI4" s="20">
         <v>621</v>
       </c>
       <c r="CJ4" s="4">
@@ -5294,12 +5063,15 @@
       </c>
       <c r="CR4" s="4">
         <v>923</v>
+      </c>
+      <c r="CS4" s="4">
+        <v>933</v>
       </c>
     </row>
     <row r="5" spans="1:231" x14ac:dyDescent="0.3">
       <c r="BP5" s="6"/>
-      <c r="CH5" s="23"/>
-      <c r="CI5" s="23"/>
+      <c r="CH5" s="19"/>
+      <c r="CI5" s="19"/>
     </row>
     <row r="6" spans="1:231" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -5465,10 +5237,10 @@
       <c r="CG6" s="4">
         <v>359</v>
       </c>
-      <c r="CH6" s="24">
+      <c r="CH6" s="20">
         <v>368</v>
       </c>
-      <c r="CI6" s="24">
+      <c r="CI6" s="20">
         <v>380</v>
       </c>
       <c r="CJ6" s="4">
@@ -5497,12 +5269,15 @@
       </c>
       <c r="CR6" s="4">
         <v>443</v>
+      </c>
+      <c r="CS6" s="4">
+        <v>448</v>
       </c>
     </row>
     <row r="7" spans="1:231" x14ac:dyDescent="0.3">
       <c r="BP7" s="6"/>
-      <c r="CH7" s="23"/>
-      <c r="CI7" s="23"/>
+      <c r="CH7" s="19"/>
+      <c r="CI7" s="19"/>
     </row>
     <row r="8" spans="1:231" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -5680,10 +5455,10 @@
       <c r="CG8" s="4">
         <v>1274</v>
       </c>
-      <c r="CH8" s="24">
+      <c r="CH8" s="20">
         <v>1347</v>
       </c>
-      <c r="CI8" s="24">
+      <c r="CI8" s="20">
         <v>1449</v>
       </c>
       <c r="CJ8" s="4">
@@ -5692,16 +5467,16 @@
       <c r="CK8" s="4">
         <v>1752</v>
       </c>
-      <c r="CL8" s="34"/>
-      <c r="CM8" s="34"/>
-      <c r="CN8" s="34"/>
-      <c r="CO8" s="34"/>
-      <c r="CP8" s="34"/>
+      <c r="CL8" s="21"/>
+      <c r="CM8" s="21"/>
+      <c r="CN8" s="21"/>
+      <c r="CO8" s="21"/>
+      <c r="CP8" s="21"/>
     </row>
     <row r="9" spans="1:231" x14ac:dyDescent="0.3">
       <c r="BP9" s="6"/>
-      <c r="CH9" s="23"/>
-      <c r="CI9" s="23"/>
+      <c r="CH9" s="19"/>
+      <c r="CI9" s="19"/>
     </row>
     <row r="10" spans="1:231" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
@@ -5806,7 +5581,7 @@
       <c r="BD10" s="13">
         <v>36</v>
       </c>
-      <c r="BE10" s="16">
+      <c r="BE10" s="15">
         <v>43</v>
       </c>
       <c r="BF10" s="13">
@@ -5827,106 +5602,108 @@
       <c r="BK10" s="11">
         <v>185</v>
       </c>
-      <c r="BL10" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="BM10" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="BN10" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="BO10" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="BP10" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="BQ10" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="BR10" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="BS10" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="BT10" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="BU10" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="BV10" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="BW10" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="BX10" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="BY10" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="BZ10" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="CA10" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="CB10" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="CC10" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="CD10" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="CE10" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="CF10" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="CG10" s="22" t="s">
-        <v>53</v>
-      </c>
-      <c r="CH10" s="25" t="s">
-        <v>54</v>
-      </c>
-      <c r="CI10" s="26" t="s">
-        <v>55</v>
-      </c>
-      <c r="CJ10" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="CK10" s="28" t="s">
-        <v>57</v>
-      </c>
-      <c r="CL10" s="29" t="s">
-        <v>58</v>
-      </c>
-      <c r="CM10" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="CN10" s="31" t="s">
-        <v>60</v>
-      </c>
-      <c r="CO10" s="32" t="s">
-        <v>61</v>
-      </c>
-      <c r="CP10" s="33" t="s">
-        <v>62</v>
-      </c>
-      <c r="CQ10" s="36" t="s">
-        <v>63</v>
-      </c>
-      <c r="CR10" s="37" t="s">
-        <v>66</v>
-      </c>
-      <c r="CS10" s="9"/>
+      <c r="BL10" s="23">
+        <v>212</v>
+      </c>
+      <c r="BM10" s="23">
+        <v>225</v>
+      </c>
+      <c r="BN10" s="23">
+        <v>235</v>
+      </c>
+      <c r="BO10" s="23">
+        <v>293</v>
+      </c>
+      <c r="BP10" s="23">
+        <v>319</v>
+      </c>
+      <c r="BQ10" s="23">
+        <v>343</v>
+      </c>
+      <c r="BR10" s="23">
+        <v>362</v>
+      </c>
+      <c r="BS10" s="23">
+        <v>407</v>
+      </c>
+      <c r="BT10" s="23">
+        <v>431</v>
+      </c>
+      <c r="BU10" s="23">
+        <v>452</v>
+      </c>
+      <c r="BV10" s="23">
+        <v>464</v>
+      </c>
+      <c r="BW10" s="23">
+        <v>523</v>
+      </c>
+      <c r="BX10" s="23">
+        <v>558</v>
+      </c>
+      <c r="BY10" s="23">
+        <v>604</v>
+      </c>
+      <c r="BZ10" s="23">
+        <v>656</v>
+      </c>
+      <c r="CA10" s="23">
+        <v>679</v>
+      </c>
+      <c r="CB10" s="23">
+        <v>697</v>
+      </c>
+      <c r="CC10" s="23">
+        <v>765</v>
+      </c>
+      <c r="CD10" s="23">
+        <v>824</v>
+      </c>
+      <c r="CE10" s="23">
+        <v>883</v>
+      </c>
+      <c r="CF10" s="23">
+        <v>905</v>
+      </c>
+      <c r="CG10" s="23">
+        <v>968</v>
+      </c>
+      <c r="CH10" s="23">
+        <v>1034</v>
+      </c>
+      <c r="CI10" s="23">
+        <v>1083</v>
+      </c>
+      <c r="CJ10" s="23">
+        <v>1149</v>
+      </c>
+      <c r="CK10" s="23">
+        <v>1200</v>
+      </c>
+      <c r="CL10" s="23">
+        <v>1250</v>
+      </c>
+      <c r="CM10" s="23">
+        <v>1278</v>
+      </c>
+      <c r="CN10" s="23">
+        <v>1342</v>
+      </c>
+      <c r="CO10" s="23">
+        <v>1387</v>
+      </c>
+      <c r="CP10" s="23">
+        <v>1405</v>
+      </c>
+      <c r="CQ10" s="23">
+        <v>1430</v>
+      </c>
+      <c r="CR10" s="23">
+        <v>1457</v>
+      </c>
+      <c r="CS10" s="11">
+        <v>1487</v>
+      </c>
       <c r="CT10" s="9"/>
       <c r="CU10" s="9"/>
       <c r="CV10" s="9"/>
@@ -6088,23 +5865,18 @@
       </c>
     </row>
     <row r="19" spans="1:1" s="6" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A19" s="15" t="s">
-        <v>64</v>
+      <c r="A19" s="14" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="72" x14ac:dyDescent="0.3">
-      <c r="A20" s="35" t="s">
-        <v>65</v>
+      <c r="A20" s="22" t="s">
+        <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" ht="228" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="17" t="s">
-        <v>49</v>
+    <row r="22" spans="1:1" ht="228" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="16" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -6202,8 +5974,8 @@
       </c>
     </row>
     <row r="5" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="18" t="s">
-        <v>47</v>
+      <c r="B5" s="17" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -6256,7 +6028,7 @@
         <v>25</v>
       </c>
       <c r="B18" t="s">
-        <v>48</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -6285,7 +6057,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>51</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Time series updated May 3
</commit_message>
<xml_diff>
--- a/data/Time_series_COVID-19_GTA_github.xlsx
+++ b/data/Time_series_COVID-19_GTA_github.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\covid-GTA-surge-planning-newrepo\covid-GTA-surge-planning\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A98A5B8-D62D-4B29-8FF9-E00CFDA0E6A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2E12FD4-4AA1-43BC-B136-AA0757FD9690}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11352" yWindow="36" windowWidth="11508" windowHeight="12072" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-168" yWindow="12" windowWidth="11508" windowHeight="12072" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Time series" sheetId="1" r:id="rId1"/>
@@ -4232,7 +4232,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="CR2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="BN1" sqref="BN1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A20" sqref="A20"/>
+      <selection pane="bottomRight" activeCell="CX2" sqref="CX2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4537,6 +4537,15 @@
       <c r="CT1" s="2">
         <v>43951</v>
       </c>
+      <c r="CU1" s="2">
+        <v>43952</v>
+      </c>
+      <c r="CV1" s="2">
+        <v>43953</v>
+      </c>
+      <c r="CW1" s="2">
+        <v>43954</v>
+      </c>
     </row>
     <row r="2" spans="1:231" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -4815,6 +4824,9 @@
       </c>
       <c r="CS2" s="12">
         <v>4845</v>
+      </c>
+      <c r="CU2" s="12">
+        <v>5230</v>
       </c>
     </row>
     <row r="3" spans="1:231" x14ac:dyDescent="0.3">
@@ -5066,6 +5078,15 @@
       </c>
       <c r="CT4" s="4">
         <v>955</v>
+      </c>
+      <c r="CU4" s="4">
+        <v>995</v>
+      </c>
+      <c r="CV4" s="4">
+        <v>1020</v>
+      </c>
+      <c r="CW4" s="4">
+        <v>1046</v>
       </c>
     </row>
     <row r="5" spans="1:231" x14ac:dyDescent="0.3">
@@ -5276,6 +5297,15 @@
       <c r="CT6" s="4">
         <v>456</v>
       </c>
+      <c r="CU6" s="4">
+        <v>461</v>
+      </c>
+      <c r="CV6" s="4">
+        <v>470</v>
+      </c>
+      <c r="CW6" s="4">
+        <v>476</v>
+      </c>
     </row>
     <row r="7" spans="1:231" x14ac:dyDescent="0.3">
       <c r="BP7" s="6"/>
@@ -5475,6 +5505,9 @@
       <c r="CN8" s="21"/>
       <c r="CO8" s="21"/>
       <c r="CP8" s="21"/>
+      <c r="CU8" s="13">
+        <v>2335</v>
+      </c>
     </row>
     <row r="9" spans="1:231" x14ac:dyDescent="0.3">
       <c r="BP9" s="6"/>
@@ -5710,9 +5743,15 @@
       <c r="CT10" s="11">
         <v>1522</v>
       </c>
-      <c r="CU10" s="9"/>
-      <c r="CV10" s="9"/>
-      <c r="CW10" s="9"/>
+      <c r="CU10" s="11">
+        <v>1568</v>
+      </c>
+      <c r="CV10" s="11">
+        <v>1612</v>
+      </c>
+      <c r="CW10" s="11">
+        <v>1639</v>
+      </c>
       <c r="CX10" s="9"/>
       <c r="CY10" s="9"/>
       <c r="CZ10" s="9"/>

</xml_diff>

<commit_message>
Time series updated May 5
</commit_message>
<xml_diff>
--- a/data/Time_series_COVID-19_GTA_github.xlsx
+++ b/data/Time_series_COVID-19_GTA_github.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\covid-GTA-surge-planning-newrepo\covid-GTA-surge-planning\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2E12FD4-4AA1-43BC-B136-AA0757FD9690}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CABF8A00-40C8-4197-9643-83E6F3233B0A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-168" yWindow="12" windowWidth="11508" windowHeight="12072" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="144" windowWidth="11508" windowHeight="12072" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Time series" sheetId="1" r:id="rId1"/>
@@ -4232,7 +4232,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="CR2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="BN1" sqref="BN1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="CX2" sqref="CX2"/>
+      <selection pane="bottomRight" activeCell="CX10" sqref="CX10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4546,6 +4546,9 @@
       <c r="CW1" s="2">
         <v>43954</v>
       </c>
+      <c r="CX1" s="2">
+        <v>43955</v>
+      </c>
     </row>
     <row r="2" spans="1:231" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -4827,6 +4830,9 @@
       </c>
       <c r="CU2" s="12">
         <v>5230</v>
+      </c>
+      <c r="CX2" s="13">
+        <v>5641</v>
       </c>
     </row>
     <row r="3" spans="1:231" x14ac:dyDescent="0.3">
@@ -5087,6 +5093,9 @@
       </c>
       <c r="CW4" s="4">
         <v>1046</v>
+      </c>
+      <c r="CX4" s="4">
+        <v>1075</v>
       </c>
     </row>
     <row r="5" spans="1:231" x14ac:dyDescent="0.3">
@@ -5306,6 +5315,9 @@
       <c r="CW6" s="4">
         <v>476</v>
       </c>
+      <c r="CX6" s="4">
+        <v>478</v>
+      </c>
     </row>
     <row r="7" spans="1:231" x14ac:dyDescent="0.3">
       <c r="BP7" s="6"/>
@@ -5752,7 +5764,9 @@
       <c r="CW10" s="11">
         <v>1639</v>
       </c>
-      <c r="CX10" s="9"/>
+      <c r="CX10" s="11">
+        <v>1656</v>
+      </c>
       <c r="CY10" s="9"/>
       <c r="CZ10" s="9"/>
       <c r="DA10" s="9"/>

</xml_diff>

<commit_message>
Time series updated May 6
</commit_message>
<xml_diff>
--- a/data/Time_series_COVID-19_GTA_github.xlsx
+++ b/data/Time_series_COVID-19_GTA_github.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\covid-GTA-surge-planning-newrepo\covid-GTA-surge-planning\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9C599A9-F1D6-4C53-A657-9F68439F58F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46BE5FAF-73CC-476E-A56F-5A1256CC3FA4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-168" yWindow="48" windowWidth="11508" windowHeight="12072" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Time series" sheetId="1" r:id="rId1"/>
@@ -4313,10 +4313,10 @@
   <dimension ref="A1:HW22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="CC2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="CW2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="BN1" sqref="BN1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="DA4" sqref="DA4"/>
+      <selection pane="bottomRight" activeCell="DA10" sqref="DA10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4636,6 +4636,9 @@
       <c r="CY1" s="2">
         <v>43956</v>
       </c>
+      <c r="CZ1" s="2">
+        <v>43957</v>
+      </c>
     </row>
     <row r="2" spans="1:231" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -4923,6 +4926,9 @@
       </c>
       <c r="CX2" s="13">
         <v>5809</v>
+      </c>
+      <c r="CY2" s="13">
+        <v>6019</v>
       </c>
     </row>
     <row r="3" spans="1:231" x14ac:dyDescent="0.3">
@@ -5189,6 +5195,9 @@
       </c>
       <c r="CY4" s="4">
         <v>1086</v>
+      </c>
+      <c r="CZ4" s="4">
+        <v>1111</v>
       </c>
     </row>
     <row r="5" spans="1:231" x14ac:dyDescent="0.3">
@@ -5414,6 +5423,9 @@
       <c r="CY6" s="4">
         <v>482</v>
       </c>
+      <c r="CZ6" s="4">
+        <v>500</v>
+      </c>
     </row>
     <row r="7" spans="1:231" x14ac:dyDescent="0.3">
       <c r="BP7" s="6"/>
@@ -5866,7 +5878,9 @@
       <c r="CY10" s="11">
         <v>1689</v>
       </c>
-      <c r="CZ10" s="9"/>
+      <c r="CZ10" s="11">
+        <v>1732</v>
+      </c>
       <c r="DA10" s="9"/>
       <c r="DB10" s="9"/>
       <c r="DC10" s="9"/>

</xml_diff>

<commit_message>
Updated time series May 7
</commit_message>
<xml_diff>
--- a/data/Time_series_COVID-19_GTA_github.xlsx
+++ b/data/Time_series_COVID-19_GTA_github.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\covid-GTA-surge-planning-newrepo\covid-GTA-surge-planning\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46BE5FAF-73CC-476E-A56F-5A1256CC3FA4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5A6AC64-F5D0-48DB-890D-50BD2FEAA5FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-168" yWindow="48" windowWidth="11508" windowHeight="12072" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="384" yWindow="288" windowWidth="11508" windowHeight="12072" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Time series" sheetId="1" r:id="rId1"/>
@@ -4316,7 +4316,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="CW2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="BN1" sqref="BN1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="DA10" sqref="DA10"/>
+      <selection pane="bottomRight" activeCell="DA11" sqref="DA11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4638,6 +4638,9 @@
       </c>
       <c r="CZ1" s="2">
         <v>43957</v>
+      </c>
+      <c r="DA1" s="2">
+        <v>43958</v>
       </c>
     </row>
     <row r="2" spans="1:231" x14ac:dyDescent="0.3">
@@ -5198,6 +5201,9 @@
       </c>
       <c r="CZ4" s="4">
         <v>1111</v>
+      </c>
+      <c r="DA4" s="4">
+        <v>1132</v>
       </c>
     </row>
     <row r="5" spans="1:231" x14ac:dyDescent="0.3">
@@ -5426,6 +5432,9 @@
       <c r="CZ6" s="4">
         <v>500</v>
       </c>
+      <c r="DA6" s="4">
+        <v>506</v>
+      </c>
     </row>
     <row r="7" spans="1:231" x14ac:dyDescent="0.3">
       <c r="BP7" s="6"/>
@@ -5881,7 +5890,9 @@
       <c r="CZ10" s="11">
         <v>1732</v>
       </c>
-      <c r="DA10" s="9"/>
+      <c r="DA10" s="11">
+        <v>1767</v>
+      </c>
       <c r="DB10" s="9"/>
       <c r="DC10" s="9"/>
       <c r="DD10" s="9"/>

</xml_diff>

<commit_message>
Updated time series May 9
</commit_message>
<xml_diff>
--- a/data/Time_series_COVID-19_GTA_github.xlsx
+++ b/data/Time_series_COVID-19_GTA_github.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\covid-GTA-surge-planning-newrepo\covid-GTA-surge-planning\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5A6AC64-F5D0-48DB-890D-50BD2FEAA5FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D952ECF-B414-44E1-89AC-B05FC88FE3F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="288" windowWidth="11508" windowHeight="12072" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1152" yWindow="288" windowWidth="11508" windowHeight="12072" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Time series" sheetId="1" r:id="rId1"/>
@@ -4316,7 +4316,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="CW2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="BN1" sqref="BN1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="DA11" sqref="DA11"/>
+      <selection pane="bottomRight" activeCell="DC11" sqref="DC11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4641,6 +4641,12 @@
       </c>
       <c r="DA1" s="2">
         <v>43958</v>
+      </c>
+      <c r="DB1" s="2">
+        <v>43959</v>
+      </c>
+      <c r="DC1" s="2">
+        <v>43960</v>
       </c>
     </row>
     <row r="2" spans="1:231" x14ac:dyDescent="0.3">
@@ -5204,6 +5210,12 @@
       </c>
       <c r="DA4" s="4">
         <v>1132</v>
+      </c>
+      <c r="DB4" s="4">
+        <v>1139</v>
+      </c>
+      <c r="DC4" s="4">
+        <v>1152</v>
       </c>
     </row>
     <row r="5" spans="1:231" x14ac:dyDescent="0.3">
@@ -5435,6 +5447,12 @@
       <c r="DA6" s="4">
         <v>506</v>
       </c>
+      <c r="DB6" s="4">
+        <v>508</v>
+      </c>
+      <c r="DC6" s="4">
+        <v>511</v>
+      </c>
     </row>
     <row r="7" spans="1:231" x14ac:dyDescent="0.3">
       <c r="BP7" s="6"/>
@@ -5893,8 +5911,12 @@
       <c r="DA10" s="11">
         <v>1767</v>
       </c>
-      <c r="DB10" s="9"/>
-      <c r="DC10" s="9"/>
+      <c r="DB10" s="11">
+        <v>1797</v>
+      </c>
+      <c r="DC10" s="11">
+        <v>1830</v>
+      </c>
       <c r="DD10" s="9"/>
       <c r="DE10" s="9"/>
       <c r="DF10" s="9"/>

</xml_diff>

<commit_message>
Time series updated May 10
</commit_message>
<xml_diff>
--- a/data/Time_series_COVID-19_GTA_github.xlsx
+++ b/data/Time_series_COVID-19_GTA_github.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\covid-GTA-surge-planning-newrepo\covid-GTA-surge-planning\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D952ECF-B414-44E1-89AC-B05FC88FE3F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{289375B0-7ECF-4A7A-871B-1413C4290D42}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="288" windowWidth="11508" windowHeight="12072" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-264" yWindow="24" windowWidth="11508" windowHeight="12072" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Time series" sheetId="1" r:id="rId1"/>
@@ -4316,7 +4316,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="CW2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="BN1" sqref="BN1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="DC11" sqref="DC11"/>
+      <selection pane="bottomRight" activeCell="DD11" sqref="DD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4647,6 +4647,9 @@
       </c>
       <c r="DC1" s="2">
         <v>43960</v>
+      </c>
+      <c r="DD1" s="2">
+        <v>43961</v>
       </c>
     </row>
     <row r="2" spans="1:231" x14ac:dyDescent="0.3">
@@ -5216,6 +5219,9 @@
       </c>
       <c r="DC4" s="4">
         <v>1152</v>
+      </c>
+      <c r="DD4" s="4">
+        <v>1162</v>
       </c>
     </row>
     <row r="5" spans="1:231" x14ac:dyDescent="0.3">
@@ -5453,6 +5459,9 @@
       <c r="DC6" s="4">
         <v>511</v>
       </c>
+      <c r="DD6" s="4">
+        <v>516</v>
+      </c>
     </row>
     <row r="7" spans="1:231" x14ac:dyDescent="0.3">
       <c r="BP7" s="6"/>
@@ -5917,7 +5926,9 @@
       <c r="DC10" s="11">
         <v>1830</v>
       </c>
-      <c r="DD10" s="9"/>
+      <c r="DD10" s="11">
+        <v>1853</v>
+      </c>
       <c r="DE10" s="9"/>
       <c r="DF10" s="9"/>
       <c r="DG10" s="9"/>

</xml_diff>

<commit_message>
Time series updated May 11
</commit_message>
<xml_diff>
--- a/data/Time_series_COVID-19_GTA_github.xlsx
+++ b/data/Time_series_COVID-19_GTA_github.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\covid-GTA-surge-planning-newrepo\covid-GTA-surge-planning\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{289375B0-7ECF-4A7A-871B-1413C4290D42}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3251DD18-DC9B-414B-89F1-0C2DCA5AAA11}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-264" yWindow="24" windowWidth="11508" windowHeight="12072" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="108" yWindow="0" windowWidth="11508" windowHeight="12072" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Time series" sheetId="1" r:id="rId1"/>
@@ -1309,13 +1309,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>97</xdr:col>
-      <xdr:colOff>274348</xdr:colOff>
+      <xdr:colOff>531523</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>171457</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>102</xdr:col>
-      <xdr:colOff>411868</xdr:colOff>
+      <xdr:col>103</xdr:col>
+      <xdr:colOff>78493</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>155223</xdr:rowOff>
     </xdr:to>
@@ -1332,7 +1332,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="19795862">
-          <a:off x="59938948" y="714382"/>
+          <a:off x="60196123" y="714382"/>
           <a:ext cx="3090270" cy="888641"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4313,10 +4313,10 @@
   <dimension ref="A1:HW22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="CW2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="CY2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="BN1" sqref="BN1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="DD11" sqref="DD11"/>
+      <selection pane="bottomRight" activeCell="DF3" sqref="DF3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4651,6 +4651,9 @@
       <c r="DD1" s="2">
         <v>43961</v>
       </c>
+      <c r="DE1" s="2">
+        <v>43962</v>
+      </c>
     </row>
     <row r="2" spans="1:231" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -4933,13 +4936,13 @@
       <c r="CU2" s="12">
         <v>5230</v>
       </c>
-      <c r="CW2" s="13">
+      <c r="CX2" s="13">
         <v>5641</v>
       </c>
-      <c r="CX2" s="13">
+      <c r="CY2" s="13">
         <v>5809</v>
       </c>
-      <c r="CY2" s="13">
+      <c r="CZ2" s="13">
         <v>6019</v>
       </c>
     </row>
@@ -5222,6 +5225,9 @@
       </c>
       <c r="DD4" s="4">
         <v>1162</v>
+      </c>
+      <c r="DE4" s="4">
+        <v>1167</v>
       </c>
     </row>
     <row r="5" spans="1:231" x14ac:dyDescent="0.3">
@@ -5929,7 +5935,9 @@
       <c r="DD10" s="11">
         <v>1853</v>
       </c>
-      <c r="DE10" s="9"/>
+      <c r="DE10" s="11">
+        <v>1905</v>
+      </c>
       <c r="DF10" s="9"/>
       <c r="DG10" s="9"/>
       <c r="DH10" s="9"/>

</xml_diff>

<commit_message>
Time series updated May 12
</commit_message>
<xml_diff>
--- a/data/Time_series_COVID-19_GTA_github.xlsx
+++ b/data/Time_series_COVID-19_GTA_github.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\covid-GTA-surge-planning-newrepo\covid-GTA-surge-planning\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3251DD18-DC9B-414B-89F1-0C2DCA5AAA11}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B094F7AC-2D56-4644-8FC6-FCB4B6845724}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="108" yWindow="0" windowWidth="11508" windowHeight="12072" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-360" yWindow="60" windowWidth="11508" windowHeight="12072" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Time series" sheetId="1" r:id="rId1"/>
@@ -4316,7 +4316,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="CY2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="BN1" sqref="BN1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="DF3" sqref="DF3"/>
+      <selection pane="bottomRight" activeCell="DF11" sqref="DF11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4653,6 +4653,9 @@
       </c>
       <c r="DE1" s="2">
         <v>43962</v>
+      </c>
+      <c r="DF1" s="2">
+        <v>43963</v>
       </c>
     </row>
     <row r="2" spans="1:231" x14ac:dyDescent="0.3">
@@ -5228,6 +5231,9 @@
       </c>
       <c r="DE4" s="4">
         <v>1167</v>
+      </c>
+      <c r="DF4" s="4">
+        <v>1176</v>
       </c>
     </row>
     <row r="5" spans="1:231" x14ac:dyDescent="0.3">
@@ -5468,6 +5474,9 @@
       <c r="DD6" s="4">
         <v>516</v>
       </c>
+      <c r="DF6" s="4">
+        <v>518</v>
+      </c>
     </row>
     <row r="7" spans="1:231" x14ac:dyDescent="0.3">
       <c r="BP7" s="6"/>
@@ -5938,7 +5947,9 @@
       <c r="DE10" s="11">
         <v>1905</v>
       </c>
-      <c r="DF10" s="9"/>
+      <c r="DF10" s="11">
+        <v>1909</v>
+      </c>
       <c r="DG10" s="9"/>
       <c r="DH10" s="9"/>
       <c r="DI10" s="9"/>

</xml_diff>

<commit_message>
Updated time series May 13
</commit_message>
<xml_diff>
--- a/data/Time_series_COVID-19_GTA_github.xlsx
+++ b/data/Time_series_COVID-19_GTA_github.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\covid-GTA-surge-planning-newrepo\covid-GTA-surge-planning\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B094F7AC-2D56-4644-8FC6-FCB4B6845724}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A040ADD-DCA1-40BF-B189-A02856BE0470}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-360" yWindow="60" windowWidth="11508" windowHeight="12072" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="768" yWindow="288" windowWidth="11508" windowHeight="12072" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Time series" sheetId="1" r:id="rId1"/>
@@ -216,7 +216,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -272,6 +272,12 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="9">
@@ -338,7 +344,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -377,6 +383,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4316,7 +4323,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="CY2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="BN1" sqref="BN1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="DF11" sqref="DF11"/>
+      <selection pane="bottomRight" activeCell="DG11" sqref="DG11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4656,6 +4663,9 @@
       </c>
       <c r="DF1" s="2">
         <v>43963</v>
+      </c>
+      <c r="DG1" s="2">
+        <v>43964</v>
       </c>
     </row>
     <row r="2" spans="1:231" x14ac:dyDescent="0.3">
@@ -5234,6 +5244,9 @@
       </c>
       <c r="DF4" s="4">
         <v>1176</v>
+      </c>
+      <c r="DG4" s="4">
+        <v>1194</v>
       </c>
     </row>
     <row r="5" spans="1:231" x14ac:dyDescent="0.3">
@@ -5477,6 +5490,9 @@
       <c r="DF6" s="4">
         <v>518</v>
       </c>
+      <c r="DG6" s="4">
+        <v>524</v>
+      </c>
     </row>
     <row r="7" spans="1:231" x14ac:dyDescent="0.3">
       <c r="BP7" s="6"/>
@@ -5950,7 +5966,9 @@
       <c r="DF10" s="11">
         <v>1909</v>
       </c>
-      <c r="DG10" s="9"/>
+      <c r="DG10" s="24">
+        <v>1939</v>
+      </c>
       <c r="DH10" s="9"/>
       <c r="DI10" s="9"/>
       <c r="DJ10" s="9"/>

</xml_diff>

<commit_message>
Time series updated May 14
</commit_message>
<xml_diff>
--- a/data/Time_series_COVID-19_GTA_github.xlsx
+++ b/data/Time_series_COVID-19_GTA_github.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\covid-GTA-surge-planning-newrepo\covid-GTA-surge-planning\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A040ADD-DCA1-40BF-B189-A02856BE0470}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{617EAC1F-6366-4547-BFEF-B05FC88882C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="288" windowWidth="11508" windowHeight="12072" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-36" yWindow="0" windowWidth="11508" windowHeight="12072" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Time series" sheetId="1" r:id="rId1"/>
@@ -4320,10 +4320,10 @@
   <dimension ref="A1:HW22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="CY2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="DB2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="BN1" sqref="BN1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="DG11" sqref="DG11"/>
+      <selection pane="bottomRight" activeCell="DH11" sqref="DH11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4666,6 +4666,9 @@
       </c>
       <c r="DG1" s="2">
         <v>43964</v>
+      </c>
+      <c r="DH1" s="2">
+        <v>43965</v>
       </c>
     </row>
     <row r="2" spans="1:231" x14ac:dyDescent="0.3">
@@ -5247,6 +5250,9 @@
       </c>
       <c r="DG4" s="4">
         <v>1194</v>
+      </c>
+      <c r="DH4" s="4">
+        <v>1201</v>
       </c>
     </row>
     <row r="5" spans="1:231" x14ac:dyDescent="0.3">
@@ -5493,6 +5499,9 @@
       <c r="DG6" s="4">
         <v>524</v>
       </c>
+      <c r="DH6" s="4">
+        <v>532</v>
+      </c>
     </row>
     <row r="7" spans="1:231" x14ac:dyDescent="0.3">
       <c r="BP7" s="6"/>
@@ -5969,7 +5978,9 @@
       <c r="DG10" s="24">
         <v>1939</v>
       </c>
-      <c r="DH10" s="9"/>
+      <c r="DH10" s="11">
+        <v>1950</v>
+      </c>
       <c r="DI10" s="9"/>
       <c r="DJ10" s="9"/>
       <c r="DK10" s="9"/>

</xml_diff>

<commit_message>
Time series updated May 16
</commit_message>
<xml_diff>
--- a/data/Time_series_COVID-19_GTA_github.xlsx
+++ b/data/Time_series_COVID-19_GTA_github.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\covid-GTA-surge-planning-newrepo\covid-GTA-surge-planning\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{617EAC1F-6366-4547-BFEF-B05FC88882C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A96C1496-DF58-415C-A966-A1FA15882980}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-36" yWindow="0" windowWidth="11508" windowHeight="12072" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-264" yWindow="0" windowWidth="11508" windowHeight="12072" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Time series" sheetId="1" r:id="rId1"/>
@@ -4323,7 +4323,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="DB2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="BN1" sqref="BN1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="DH11" sqref="DH11"/>
+      <selection pane="bottomRight" activeCell="DJ11" sqref="DJ11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4669,6 +4669,12 @@
       </c>
       <c r="DH1" s="2">
         <v>43965</v>
+      </c>
+      <c r="DI1" s="2">
+        <v>43966</v>
+      </c>
+      <c r="DJ1" s="2">
+        <v>43967</v>
       </c>
     </row>
     <row r="2" spans="1:231" x14ac:dyDescent="0.3">
@@ -5253,6 +5259,12 @@
       </c>
       <c r="DH4" s="4">
         <v>1201</v>
+      </c>
+      <c r="DI4" s="4">
+        <v>1212</v>
+      </c>
+      <c r="DJ4" s="4">
+        <v>1226</v>
       </c>
     </row>
     <row r="5" spans="1:231" x14ac:dyDescent="0.3">
@@ -5502,6 +5514,12 @@
       <c r="DH6" s="4">
         <v>532</v>
       </c>
+      <c r="DI6" s="4">
+        <v>557</v>
+      </c>
+      <c r="DJ6" s="4">
+        <v>563</v>
+      </c>
     </row>
     <row r="7" spans="1:231" x14ac:dyDescent="0.3">
       <c r="BP7" s="6"/>
@@ -5981,8 +5999,12 @@
       <c r="DH10" s="11">
         <v>1950</v>
       </c>
-      <c r="DI10" s="9"/>
-      <c r="DJ10" s="9"/>
+      <c r="DI10" s="11">
+        <v>1973</v>
+      </c>
+      <c r="DJ10" s="11">
+        <v>1994</v>
+      </c>
       <c r="DK10" s="9"/>
       <c r="DL10" s="9"/>
       <c r="DM10" s="9"/>

</xml_diff>

<commit_message>
Time series updated May 17
</commit_message>
<xml_diff>
--- a/data/Time_series_COVID-19_GTA_github.xlsx
+++ b/data/Time_series_COVID-19_GTA_github.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\covid-GTA-surge-planning-newrepo\covid-GTA-surge-planning\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A96C1496-DF58-415C-A966-A1FA15882980}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76AD631B-C317-481F-B523-D7483D5FE1DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-264" yWindow="0" windowWidth="11508" windowHeight="12072" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11508" windowHeight="12072" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Time series" sheetId="1" r:id="rId1"/>
@@ -4320,10 +4320,10 @@
   <dimension ref="A1:HW22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="DB2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="DE2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="BN1" sqref="BN1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="DJ11" sqref="DJ11"/>
+      <selection pane="bottomRight" activeCell="DK7" sqref="DK7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4675,6 +4675,9 @@
       </c>
       <c r="DJ1" s="2">
         <v>43967</v>
+      </c>
+      <c r="DK1" s="2">
+        <v>43968</v>
       </c>
     </row>
     <row r="2" spans="1:231" x14ac:dyDescent="0.3">
@@ -5265,6 +5268,9 @@
       </c>
       <c r="DJ4" s="4">
         <v>1226</v>
+      </c>
+      <c r="DK4" s="4">
+        <v>1245</v>
       </c>
     </row>
     <row r="5" spans="1:231" x14ac:dyDescent="0.3">
@@ -5515,9 +5521,12 @@
         <v>532</v>
       </c>
       <c r="DI6" s="4">
+        <v>550</v>
+      </c>
+      <c r="DJ6" s="4">
         <v>557</v>
       </c>
-      <c r="DJ6" s="4">
+      <c r="DK6" s="4">
         <v>563</v>
       </c>
     </row>
@@ -6005,7 +6014,9 @@
       <c r="DJ10" s="11">
         <v>1994</v>
       </c>
-      <c r="DK10" s="9"/>
+      <c r="DK10" s="11">
+        <v>2038</v>
+      </c>
       <c r="DL10" s="9"/>
       <c r="DM10" s="9"/>
       <c r="DN10" s="9"/>

</xml_diff>

<commit_message>
Time series updated May 18
</commit_message>
<xml_diff>
--- a/data/Time_series_COVID-19_GTA_github.xlsx
+++ b/data/Time_series_COVID-19_GTA_github.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\covid-GTA-surge-planning-newrepo\covid-GTA-surge-planning\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76AD631B-C317-481F-B523-D7483D5FE1DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79905C20-0E1C-4B78-8559-007F4611EE1E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11508" windowHeight="12072" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-84" yWindow="0" windowWidth="11508" windowHeight="12072" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Time series" sheetId="1" r:id="rId1"/>
@@ -4323,7 +4323,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="DE2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="BN1" sqref="BN1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="DK7" sqref="DK7"/>
+      <selection pane="bottomRight" activeCell="DL11" sqref="DL11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4678,6 +4678,9 @@
       </c>
       <c r="DK1" s="2">
         <v>43968</v>
+      </c>
+      <c r="DL1" s="2">
+        <v>43969</v>
       </c>
     </row>
     <row r="2" spans="1:231" x14ac:dyDescent="0.3">
@@ -5271,6 +5274,9 @@
       </c>
       <c r="DK4" s="4">
         <v>1245</v>
+      </c>
+      <c r="DL4" s="4">
+        <v>1266</v>
       </c>
     </row>
     <row r="5" spans="1:231" x14ac:dyDescent="0.3">
@@ -5529,6 +5535,9 @@
       <c r="DK6" s="4">
         <v>563</v>
       </c>
+      <c r="DL6" s="4">
+        <v>577</v>
+      </c>
     </row>
     <row r="7" spans="1:231" x14ac:dyDescent="0.3">
       <c r="BP7" s="6"/>
@@ -6017,7 +6026,9 @@
       <c r="DK10" s="11">
         <v>2038</v>
       </c>
-      <c r="DL10" s="9"/>
+      <c r="DL10" s="11">
+        <v>2056</v>
+      </c>
       <c r="DM10" s="9"/>
       <c r="DN10" s="9"/>
       <c r="DO10" s="9"/>

</xml_diff>

<commit_message>
Time series updated May 19
</commit_message>
<xml_diff>
--- a/data/Time_series_COVID-19_GTA_github.xlsx
+++ b/data/Time_series_COVID-19_GTA_github.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\covid-GTA-surge-planning-newrepo\covid-GTA-surge-planning\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79905C20-0E1C-4B78-8559-007F4611EE1E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC16CB79-21A8-411B-9201-7B3AB3B73C89}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-84" yWindow="0" windowWidth="11508" windowHeight="12072" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Time series" sheetId="1" r:id="rId1"/>
@@ -1397,6 +1397,90 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>108</xdr:col>
+      <xdr:colOff>341023</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>171457</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>113</xdr:col>
+      <xdr:colOff>478543</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>155223</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="20" name="CustomShape 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F38B1E70-22FD-4CC4-9F4A-02C1F43EBE83}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="19795862">
+          <a:off x="66501673" y="714382"/>
+          <a:ext cx="3090270" cy="888641"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr>
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="5400" b="1" strike="noStrike" spc="-1">
+              <a:solidFill>
+                <a:srgbClr val="7C7C7C">
+                  <a:alpha val="50000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:latin typeface="Times New Roman"/>
+            </a:rPr>
+            <a:t>DRAFT</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="5400" b="0" strike="noStrike" spc="-1">
+            <a:solidFill>
+              <a:srgbClr val="7C7C7C">
+                <a:alpha val="50000"/>
+              </a:srgbClr>
+            </a:solidFill>
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -4320,10 +4404,10 @@
   <dimension ref="A1:HW22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="DE2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="CU2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="BN1" sqref="BN1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="DL11" sqref="DL11"/>
+      <selection pane="bottomRight" activeCell="DM11" sqref="DM11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4681,6 +4765,9 @@
       </c>
       <c r="DL1" s="2">
         <v>43969</v>
+      </c>
+      <c r="DM1" s="2">
+        <v>43970</v>
       </c>
     </row>
     <row r="2" spans="1:231" x14ac:dyDescent="0.3">
@@ -5277,6 +5364,9 @@
       </c>
       <c r="DL4" s="4">
         <v>1266</v>
+      </c>
+      <c r="DM4" s="4">
+        <v>1285</v>
       </c>
     </row>
     <row r="5" spans="1:231" x14ac:dyDescent="0.3">
@@ -5538,6 +5628,9 @@
       <c r="DL6" s="4">
         <v>577</v>
       </c>
+      <c r="DM6" s="4">
+        <v>587</v>
+      </c>
     </row>
     <row r="7" spans="1:231" x14ac:dyDescent="0.3">
       <c r="BP7" s="6"/>
@@ -6029,7 +6122,9 @@
       <c r="DL10" s="11">
         <v>2056</v>
       </c>
-      <c r="DM10" s="9"/>
+      <c r="DM10" s="11">
+        <v>2080</v>
+      </c>
       <c r="DN10" s="9"/>
       <c r="DO10" s="9"/>
       <c r="DP10" s="9"/>

</xml_diff>

<commit_message>
Time series updated May 20
</commit_message>
<xml_diff>
--- a/data/Time_series_COVID-19_GTA_github.xlsx
+++ b/data/Time_series_COVID-19_GTA_github.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\covid-GTA-surge-planning-newrepo\covid-GTA-surge-planning\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC16CB79-21A8-411B-9201-7B3AB3B73C89}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98C9D211-E02D-42D0-8F96-9E240C32415A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-648" yWindow="0" windowWidth="11508" windowHeight="12072" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Time series" sheetId="1" r:id="rId1"/>
@@ -4404,10 +4404,10 @@
   <dimension ref="A1:HW22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="CU2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="DG2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="BN1" sqref="BN1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="DM11" sqref="DM11"/>
+      <selection pane="bottomRight" activeCell="DN11" sqref="DN11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4768,6 +4768,9 @@
       </c>
       <c r="DM1" s="2">
         <v>43970</v>
+      </c>
+      <c r="DN1" s="2">
+        <v>43971</v>
       </c>
     </row>
     <row r="2" spans="1:231" x14ac:dyDescent="0.3">
@@ -5367,6 +5370,9 @@
       </c>
       <c r="DM4" s="4">
         <v>1285</v>
+      </c>
+      <c r="DN4" s="4">
+        <v>1295</v>
       </c>
     </row>
     <row r="5" spans="1:231" x14ac:dyDescent="0.3">
@@ -5631,6 +5637,9 @@
       <c r="DM6" s="4">
         <v>587</v>
       </c>
+      <c r="DN6" s="4">
+        <v>587</v>
+      </c>
     </row>
     <row r="7" spans="1:231" x14ac:dyDescent="0.3">
       <c r="BP7" s="6"/>
@@ -6125,7 +6134,9 @@
       <c r="DM10" s="11">
         <v>2080</v>
       </c>
-      <c r="DN10" s="9"/>
+      <c r="DN10" s="11">
+        <v>2115</v>
+      </c>
       <c r="DO10" s="9"/>
       <c r="DP10" s="9"/>
       <c r="DQ10" s="9"/>

</xml_diff>

<commit_message>
Time series updated May 21
</commit_message>
<xml_diff>
--- a/data/Time_series_COVID-19_GTA_github.xlsx
+++ b/data/Time_series_COVID-19_GTA_github.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\covid-GTA-surge-planning-newrepo\covid-GTA-surge-planning\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98C9D211-E02D-42D0-8F96-9E240C32415A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35ACE9FC-187B-4F7A-BC0F-C0D8603532C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-648" yWindow="0" windowWidth="11508" windowHeight="12072" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="768" yWindow="288" windowWidth="11508" windowHeight="12072" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Time series" sheetId="1" r:id="rId1"/>
@@ -4407,7 +4407,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="DG2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="BN1" sqref="BN1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="DN11" sqref="DN11"/>
+      <selection pane="bottomRight" activeCell="DO5" sqref="DO5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4771,6 +4771,9 @@
       </c>
       <c r="DN1" s="2">
         <v>43971</v>
+      </c>
+      <c r="DO1" s="2">
+        <v>43972</v>
       </c>
     </row>
     <row r="2" spans="1:231" x14ac:dyDescent="0.3">
@@ -5373,6 +5376,9 @@
       </c>
       <c r="DN4" s="4">
         <v>1295</v>
+      </c>
+      <c r="DO4" s="4">
+        <v>1318</v>
       </c>
     </row>
     <row r="5" spans="1:231" x14ac:dyDescent="0.3">
@@ -5640,6 +5646,9 @@
       <c r="DN6" s="4">
         <v>587</v>
       </c>
+      <c r="DO6" s="4">
+        <v>595</v>
+      </c>
     </row>
     <row r="7" spans="1:231" x14ac:dyDescent="0.3">
       <c r="BP7" s="6"/>
@@ -6137,7 +6146,9 @@
       <c r="DN10" s="11">
         <v>2115</v>
       </c>
-      <c r="DO10" s="9"/>
+      <c r="DO10" s="11">
+        <v>2142</v>
+      </c>
       <c r="DP10" s="9"/>
       <c r="DQ10" s="9"/>
       <c r="DR10" s="9"/>

</xml_diff>

<commit_message>
Time series updated May 23
</commit_message>
<xml_diff>
--- a/data/Time_series_COVID-19_GTA_github.xlsx
+++ b/data/Time_series_COVID-19_GTA_github.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\covid-GTA-surge-planning-newrepo\covid-GTA-surge-planning\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35ACE9FC-187B-4F7A-BC0F-C0D8603532C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7805ADC0-1922-4FEB-B5E0-DD92223DE980}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="288" windowWidth="11508" windowHeight="12072" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="144" yWindow="0" windowWidth="11508" windowHeight="12072" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Time series" sheetId="1" r:id="rId1"/>
@@ -4404,10 +4404,10 @@
   <dimension ref="A1:HW22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="DG2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="DL2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="BN1" sqref="BN1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="DO5" sqref="DO5"/>
+      <selection pane="bottomRight" activeCell="DQ10" sqref="DQ10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4774,6 +4774,12 @@
       </c>
       <c r="DO1" s="2">
         <v>43972</v>
+      </c>
+      <c r="DP1" s="2">
+        <v>43973</v>
+      </c>
+      <c r="DQ1" s="2">
+        <v>43974</v>
       </c>
     </row>
     <row r="2" spans="1:231" x14ac:dyDescent="0.3">
@@ -5379,6 +5385,12 @@
       </c>
       <c r="DO4" s="4">
         <v>1318</v>
+      </c>
+      <c r="DP4" s="4">
+        <v>1324</v>
+      </c>
+      <c r="DQ4" s="4">
+        <v>1342</v>
       </c>
     </row>
     <row r="5" spans="1:231" x14ac:dyDescent="0.3">
@@ -5649,6 +5661,12 @@
       <c r="DO6" s="4">
         <v>595</v>
       </c>
+      <c r="DP6" s="4">
+        <v>606</v>
+      </c>
+      <c r="DQ6" s="4">
+        <v>610</v>
+      </c>
     </row>
     <row r="7" spans="1:231" x14ac:dyDescent="0.3">
       <c r="BP7" s="6"/>
@@ -5851,6 +5869,15 @@
       <c r="CU8" s="13">
         <v>2335</v>
       </c>
+      <c r="DB8" s="13">
+        <v>2732</v>
+      </c>
+      <c r="DI8" s="13">
+        <v>3157</v>
+      </c>
+      <c r="DP8" s="13">
+        <v>3610</v>
+      </c>
     </row>
     <row r="9" spans="1:231" x14ac:dyDescent="0.3">
       <c r="BP9" s="6"/>
@@ -6149,8 +6176,12 @@
       <c r="DO10" s="11">
         <v>2142</v>
       </c>
-      <c r="DP10" s="9"/>
-      <c r="DQ10" s="9"/>
+      <c r="DP10" s="11">
+        <v>2191</v>
+      </c>
+      <c r="DQ10" s="11">
+        <v>2230</v>
+      </c>
       <c r="DR10" s="9"/>
       <c r="DS10" s="9"/>
       <c r="DT10" s="9"/>

</xml_diff>

<commit_message>
Time series updatd May 24
</commit_message>
<xml_diff>
--- a/data/Time_series_COVID-19_GTA_github.xlsx
+++ b/data/Time_series_COVID-19_GTA_github.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\covid-GTA-surge-planning-newrepo\covid-GTA-surge-planning\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7805ADC0-1922-4FEB-B5E0-DD92223DE980}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8E1D338-A5EE-471B-A25E-B94638634B25}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="144" yWindow="0" windowWidth="11508" windowHeight="12072" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="264" yWindow="48" windowWidth="11508" windowHeight="12072" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Time series" sheetId="1" r:id="rId1"/>
@@ -4407,7 +4407,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="DL2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="BN1" sqref="BN1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="DQ10" sqref="DQ10"/>
+      <selection pane="bottomRight" activeCell="DR11" sqref="DR11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4780,6 +4780,9 @@
       </c>
       <c r="DQ1" s="2">
         <v>43974</v>
+      </c>
+      <c r="DR1" s="2">
+        <v>43975</v>
       </c>
     </row>
     <row r="2" spans="1:231" x14ac:dyDescent="0.3">
@@ -5391,6 +5394,9 @@
       </c>
       <c r="DQ4" s="4">
         <v>1342</v>
+      </c>
+      <c r="DR4" s="4">
+        <v>1358</v>
       </c>
     </row>
     <row r="5" spans="1:231" x14ac:dyDescent="0.3">
@@ -5667,6 +5673,9 @@
       <c r="DQ6" s="4">
         <v>610</v>
       </c>
+      <c r="DR6" s="4">
+        <v>612</v>
+      </c>
     </row>
     <row r="7" spans="1:231" x14ac:dyDescent="0.3">
       <c r="BP7" s="6"/>
@@ -6182,7 +6191,9 @@
       <c r="DQ10" s="11">
         <v>2230</v>
       </c>
-      <c r="DR10" s="9"/>
+      <c r="DR10" s="11">
+        <v>2260</v>
+      </c>
       <c r="DS10" s="9"/>
       <c r="DT10" s="9"/>
       <c r="DU10" s="9"/>

</xml_diff>

<commit_message>
Time series updated May 27
</commit_message>
<xml_diff>
--- a/data/Time_series_COVID-19_GTA_github.xlsx
+++ b/data/Time_series_COVID-19_GTA_github.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\covid-GTA-surge-planning-newrepo\covid-GTA-surge-planning\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09F980DF-EF95-484F-952C-29F5BAFFDDFF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34444C12-4A1B-4F9D-8568-CE8C0E955749}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="0" windowWidth="11508" windowHeight="12072" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-372" yWindow="0" windowWidth="11508" windowHeight="12072" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Time series" sheetId="1" r:id="rId1"/>
@@ -4404,10 +4404,10 @@
   <dimension ref="A1:HW22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="DL2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="DO2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="BN1" sqref="BN1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="DT11" sqref="DT11"/>
+      <selection pane="bottomRight" activeCell="DU10" sqref="DU10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4790,6 +4790,10 @@
       <c r="DT1" s="2">
         <v>43977</v>
       </c>
+      <c r="DU1" s="2">
+        <v>43978</v>
+      </c>
+      <c r="DV1" s="2"/>
     </row>
     <row r="2" spans="1:231" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -5409,6 +5413,9 @@
       </c>
       <c r="DT4" s="4">
         <v>1399</v>
+      </c>
+      <c r="DU4" s="4">
+        <v>1404</v>
       </c>
     </row>
     <row r="5" spans="1:231" x14ac:dyDescent="0.3">
@@ -5694,6 +5701,9 @@
       <c r="DT6" s="4">
         <v>623</v>
       </c>
+      <c r="DU6" s="4">
+        <v>628</v>
+      </c>
     </row>
     <row r="7" spans="1:231" x14ac:dyDescent="0.3">
       <c r="BP7" s="6"/>
@@ -6218,7 +6228,9 @@
       <c r="DT10" s="11">
         <v>2308</v>
       </c>
-      <c r="DU10" s="9"/>
+      <c r="DU10" s="11">
+        <v>2343</v>
+      </c>
       <c r="DV10" s="9"/>
       <c r="DW10" s="9"/>
       <c r="DX10" s="9"/>

</xml_diff>

<commit_message>
Time series updated May 30
</commit_message>
<xml_diff>
--- a/data/Time_series_COVID-19_GTA_github.xlsx
+++ b/data/Time_series_COVID-19_GTA_github.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\covid-GTA-surge-planning-newrepo\covid-GTA-surge-planning\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B002E3F8-28EC-4A01-87AE-5C162F3C84CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0D8A479-C999-4C11-9ADF-BDB800CA3CCE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="288" windowWidth="11508" windowHeight="12072" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-72" yWindow="0" windowWidth="11508" windowHeight="12072" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Time series" sheetId="1" r:id="rId1"/>
@@ -4407,7 +4407,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="DP2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="BN1" sqref="BN1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="DX10" sqref="DX10"/>
+      <selection pane="bottomRight" activeCell="DX8" sqref="DX8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4798,6 +4798,9 @@
       </c>
       <c r="DW1" s="2">
         <v>43980</v>
+      </c>
+      <c r="DX1" s="2">
+        <v>43981</v>
       </c>
     </row>
     <row r="2" spans="1:231" x14ac:dyDescent="0.3">
@@ -5427,6 +5430,9 @@
       </c>
       <c r="DW4" s="4">
         <v>1435</v>
+      </c>
+      <c r="DX4" s="4">
+        <v>1449</v>
       </c>
     </row>
     <row r="5" spans="1:231" x14ac:dyDescent="0.3">
@@ -5721,6 +5727,9 @@
       <c r="DW6" s="4">
         <v>635</v>
       </c>
+      <c r="DX6" s="4">
+        <v>640</v>
+      </c>
     </row>
     <row r="7" spans="1:231" x14ac:dyDescent="0.3">
       <c r="BP7" s="6"/>
@@ -5932,6 +5941,9 @@
       <c r="DP8" s="13">
         <v>3610</v>
       </c>
+      <c r="DW8" s="13">
+        <v>4193</v>
+      </c>
     </row>
     <row r="9" spans="1:231" x14ac:dyDescent="0.3">
       <c r="BP9" s="6"/>
@@ -6254,7 +6266,9 @@
       <c r="DW10" s="11">
         <v>2384</v>
       </c>
-      <c r="DX10" s="9"/>
+      <c r="DX10" s="11">
+        <v>2412</v>
+      </c>
       <c r="DY10" s="9"/>
       <c r="DZ10" s="9"/>
       <c r="EA10" s="9"/>

</xml_diff>

<commit_message>
Time series updated May 31
</commit_message>
<xml_diff>
--- a/data/Time_series_COVID-19_GTA_github.xlsx
+++ b/data/Time_series_COVID-19_GTA_github.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\covid-GTA-surge-planning-newrepo\covid-GTA-surge-planning\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0D8A479-C999-4C11-9ADF-BDB800CA3CCE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF282970-EE97-4868-8E56-76B244773CFE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-72" yWindow="0" windowWidth="11508" windowHeight="12072" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="168" yWindow="0" windowWidth="11508" windowHeight="12072" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Time series" sheetId="1" r:id="rId1"/>
@@ -4404,10 +4404,10 @@
   <dimension ref="A1:HW22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="DP2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="DS2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="BN1" sqref="BN1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="DX8" sqref="DX8"/>
+      <selection pane="bottomRight" activeCell="DY10" sqref="DY10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4802,6 +4802,10 @@
       <c r="DX1" s="2">
         <v>43981</v>
       </c>
+      <c r="DY1" s="2">
+        <v>43982</v>
+      </c>
+      <c r="DZ1" s="2"/>
     </row>
     <row r="2" spans="1:231" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -5433,6 +5437,9 @@
       </c>
       <c r="DX4" s="4">
         <v>1449</v>
+      </c>
+      <c r="DY4" s="4">
+        <v>1462</v>
       </c>
     </row>
     <row r="5" spans="1:231" x14ac:dyDescent="0.3">
@@ -5730,6 +5737,9 @@
       <c r="DX6" s="4">
         <v>640</v>
       </c>
+      <c r="DY6" s="4">
+        <v>643</v>
+      </c>
     </row>
     <row r="7" spans="1:231" x14ac:dyDescent="0.3">
       <c r="BP7" s="6"/>
@@ -6269,7 +6279,9 @@
       <c r="DX10" s="11">
         <v>2412</v>
       </c>
-      <c r="DY10" s="9"/>
+      <c r="DY10" s="11">
+        <v>2434</v>
+      </c>
       <c r="DZ10" s="9"/>
       <c r="EA10" s="9"/>
       <c r="EB10" s="9"/>

</xml_diff>

<commit_message>
Time series updated June 1
</commit_message>
<xml_diff>
--- a/data/Time_series_COVID-19_GTA_github.xlsx
+++ b/data/Time_series_COVID-19_GTA_github.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\covid-GTA-surge-planning-newrepo\covid-GTA-surge-planning\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF282970-EE97-4868-8E56-76B244773CFE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C35CECF8-C252-4977-A4D6-12DE77630C55}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="168" yWindow="0" windowWidth="11508" windowHeight="12072" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="384" yWindow="288" windowWidth="11508" windowHeight="12072" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Time series" sheetId="1" r:id="rId1"/>
@@ -4407,7 +4407,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="DS2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="BN1" sqref="BN1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="DY10" sqref="DY10"/>
+      <selection pane="bottomRight" activeCell="DZ11" sqref="DZ11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4805,7 +4805,9 @@
       <c r="DY1" s="2">
         <v>43982</v>
       </c>
-      <c r="DZ1" s="2"/>
+      <c r="DZ1" s="2">
+        <v>43983</v>
+      </c>
     </row>
     <row r="2" spans="1:231" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -5440,6 +5442,9 @@
       </c>
       <c r="DY4" s="4">
         <v>1462</v>
+      </c>
+      <c r="DZ4" s="4">
+        <v>1472</v>
       </c>
     </row>
     <row r="5" spans="1:231" x14ac:dyDescent="0.3">
@@ -5740,6 +5745,9 @@
       <c r="DY6" s="4">
         <v>643</v>
       </c>
+      <c r="DZ6" s="4">
+        <v>645</v>
+      </c>
     </row>
     <row r="7" spans="1:231" x14ac:dyDescent="0.3">
       <c r="BP7" s="6"/>
@@ -6282,7 +6290,9 @@
       <c r="DY10" s="11">
         <v>2434</v>
       </c>
-      <c r="DZ10" s="9"/>
+      <c r="DZ10" s="11">
+        <v>2464</v>
+      </c>
       <c r="EA10" s="9"/>
       <c r="EB10" s="9"/>
       <c r="EC10" s="9"/>

</xml_diff>

<commit_message>
Time series updated June 3
</commit_message>
<xml_diff>
--- a/data/Time_series_COVID-19_GTA_github.xlsx
+++ b/data/Time_series_COVID-19_GTA_github.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\covid-GTA-surge-planning-newrepo\covid-GTA-surge-planning\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C35CECF8-C252-4977-A4D6-12DE77630C55}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2079BE6-E4BA-41E4-924E-6D20DB92D106}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="288" windowWidth="11508" windowHeight="12072" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="384" yWindow="48" windowWidth="11508" windowHeight="12072" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Time series" sheetId="1" r:id="rId1"/>
@@ -4404,10 +4404,10 @@
   <dimension ref="A1:HW22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="DS2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="DU2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="BN1" sqref="BN1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="DZ11" sqref="DZ11"/>
+      <selection pane="bottomRight" activeCell="EB11" sqref="EB11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4807,6 +4807,12 @@
       </c>
       <c r="DZ1" s="2">
         <v>43983</v>
+      </c>
+      <c r="EA1" s="2">
+        <v>43984</v>
+      </c>
+      <c r="EB1" s="2">
+        <v>43985</v>
       </c>
     </row>
     <row r="2" spans="1:231" x14ac:dyDescent="0.3">
@@ -5445,6 +5451,12 @@
       </c>
       <c r="DZ4" s="4">
         <v>1472</v>
+      </c>
+      <c r="EA4" s="4">
+        <v>1489</v>
+      </c>
+      <c r="EB4" s="4">
+        <v>1500</v>
       </c>
     </row>
     <row r="5" spans="1:231" x14ac:dyDescent="0.3">
@@ -5748,6 +5760,12 @@
       <c r="DZ6" s="4">
         <v>645</v>
       </c>
+      <c r="EA6" s="4">
+        <v>649</v>
+      </c>
+      <c r="EB6" s="4">
+        <v>649</v>
+      </c>
     </row>
     <row r="7" spans="1:231" x14ac:dyDescent="0.3">
       <c r="BP7" s="6"/>
@@ -6293,8 +6311,12 @@
       <c r="DZ10" s="11">
         <v>2464</v>
       </c>
-      <c r="EA10" s="9"/>
-      <c r="EB10" s="9"/>
+      <c r="EA10" s="11">
+        <v>2515</v>
+      </c>
+      <c r="EB10" s="11">
+        <v>2567</v>
+      </c>
       <c r="EC10" s="9"/>
       <c r="ED10" s="9"/>
       <c r="EE10" s="9"/>

</xml_diff>

<commit_message>
Time series updated June 7
</commit_message>
<xml_diff>
--- a/data/Time_series_COVID-19_GTA_github.xlsx
+++ b/data/Time_series_COVID-19_GTA_github.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\covid-GTA-surge-planning-newrepo\covid-GTA-surge-planning\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2079BE6-E4BA-41E4-924E-6D20DB92D106}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{467D7426-A257-4ED1-B3B1-067AAC7D7B6D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="48" windowWidth="11508" windowHeight="12072" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Time series" sheetId="1" r:id="rId1"/>
@@ -1481,6 +1481,174 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>119</xdr:col>
+      <xdr:colOff>207673</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>38107</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>124</xdr:col>
+      <xdr:colOff>345193</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>21873</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="21" name="CustomShape 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{46675C4C-E32F-4C50-9AAA-B24098D0FD7C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="19795862">
+          <a:off x="72864373" y="762007"/>
+          <a:ext cx="3090270" cy="888641"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr>
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="5400" b="1" strike="noStrike" spc="-1">
+              <a:solidFill>
+                <a:srgbClr val="7C7C7C">
+                  <a:alpha val="50000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:latin typeface="Times New Roman"/>
+            </a:rPr>
+            <a:t>DRAFT</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="5400" b="0" strike="noStrike" spc="-1">
+            <a:solidFill>
+              <a:srgbClr val="7C7C7C">
+                <a:alpha val="50000"/>
+              </a:srgbClr>
+            </a:solidFill>
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>130</xdr:col>
+      <xdr:colOff>398173</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>171457</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>135</xdr:col>
+      <xdr:colOff>535693</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>155223</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="22" name="CustomShape 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F5677B77-D063-432E-96CB-82CC884097EE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="19795862">
+          <a:off x="79550923" y="714382"/>
+          <a:ext cx="3090270" cy="888641"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr>
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="5400" b="1" strike="noStrike" spc="-1">
+              <a:solidFill>
+                <a:srgbClr val="7C7C7C">
+                  <a:alpha val="50000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:latin typeface="Times New Roman"/>
+            </a:rPr>
+            <a:t>DRAFT</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="5400" b="0" strike="noStrike" spc="-1">
+            <a:solidFill>
+              <a:srgbClr val="7C7C7C">
+                <a:alpha val="50000"/>
+              </a:srgbClr>
+            </a:solidFill>
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -4404,10 +4572,10 @@
   <dimension ref="A1:HW22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="DU2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="DK2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="BN1" sqref="BN1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="EB11" sqref="EB11"/>
+      <selection pane="bottomRight" activeCell="ED8" sqref="ED8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4813,6 +4981,18 @@
       </c>
       <c r="EB1" s="2">
         <v>43985</v>
+      </c>
+      <c r="EC1" s="2">
+        <v>43986</v>
+      </c>
+      <c r="ED1" s="2">
+        <v>43987</v>
+      </c>
+      <c r="EE1" s="2">
+        <v>43988</v>
+      </c>
+      <c r="EF1" s="2">
+        <v>43989</v>
       </c>
     </row>
     <row r="2" spans="1:231" x14ac:dyDescent="0.3">
@@ -5457,6 +5637,18 @@
       </c>
       <c r="EB4" s="4">
         <v>1500</v>
+      </c>
+      <c r="EC4" s="4">
+        <v>1519</v>
+      </c>
+      <c r="ED4" s="4">
+        <v>1558</v>
+      </c>
+      <c r="EE4" s="4">
+        <v>1562</v>
+      </c>
+      <c r="EF4" s="4">
+        <v>1576</v>
       </c>
     </row>
     <row r="5" spans="1:231" x14ac:dyDescent="0.3">
@@ -5766,6 +5958,18 @@
       <c r="EB6" s="4">
         <v>649</v>
       </c>
+      <c r="EC6" s="4">
+        <v>661</v>
+      </c>
+      <c r="ED6" s="4">
+        <v>666</v>
+      </c>
+      <c r="EE6" s="4">
+        <v>667</v>
+      </c>
+      <c r="EF6" s="4">
+        <v>670</v>
+      </c>
     </row>
     <row r="7" spans="1:231" x14ac:dyDescent="0.3">
       <c r="BP7" s="6"/>
@@ -5980,6 +6184,9 @@
       <c r="DW8" s="13">
         <v>4193</v>
       </c>
+      <c r="ED8" s="13">
+        <v>4762</v>
+      </c>
     </row>
     <row r="9" spans="1:231" x14ac:dyDescent="0.3">
       <c r="BP9" s="6"/>
@@ -6317,10 +6524,18 @@
       <c r="EB10" s="11">
         <v>2567</v>
       </c>
-      <c r="EC10" s="9"/>
-      <c r="ED10" s="9"/>
-      <c r="EE10" s="9"/>
-      <c r="EF10" s="9"/>
+      <c r="EC10" s="11">
+        <v>2581</v>
+      </c>
+      <c r="ED10" s="11">
+        <v>2602</v>
+      </c>
+      <c r="EE10" s="11">
+        <v>2617</v>
+      </c>
+      <c r="EF10" s="11">
+        <v>2628</v>
+      </c>
       <c r="EG10" s="9"/>
       <c r="EH10" s="9"/>
       <c r="EI10" s="9"/>

</xml_diff>